<commit_message>
fixing date changes, parameter re-ordering etc
</commit_message>
<xml_diff>
--- a/LUSID Excel - Setting up your market data.xlsx
+++ b/LUSID Excel - Setting up your market data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://finbourne.sharepoint.com/Shared Documents/Product/CustomerProposition/Getting started tutorials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusSekhon\Dev\sample-excel\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{B32354FE-22B9-454E-9DB0-CA4823A7F011}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9F843045-B59F-43B8-950A-2325F65DF894}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A469E-386C-4456-8F6D-8235C1B74DB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Datetime format" sheetId="18" r:id="rId1"/>
+    <sheet name="Datetime format" sheetId="21" r:id="rId1"/>
     <sheet name="List identifiers" sheetId="11" r:id="rId2"/>
     <sheet name="List instruments" sheetId="12" r:id="rId3"/>
     <sheet name="Get instrument definition" sheetId="10" r:id="rId4"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="333">
   <si>
     <t>Base Currency</t>
   </si>
@@ -936,33 +936,18 @@
     <t>or Contact us</t>
   </si>
   <si>
-    <t>Excel format</t>
-  </si>
-  <si>
-    <t>LUSID format</t>
-  </si>
-  <si>
     <t>Enter the date to convert</t>
   </si>
   <si>
-    <t>LUSID requires dates in the following format:</t>
-  </si>
-  <si>
     <t>This date has no time component</t>
   </si>
   <si>
-    <t>Convert into a string (no time component):</t>
-  </si>
-  <si>
     <t>Specify time component</t>
   </si>
   <si>
     <t>Add to your date and display the complete datetime</t>
   </si>
   <si>
-    <t>Convert into a string (time component):</t>
-  </si>
-  <si>
     <t>Although the date can still appears without time</t>
   </si>
   <si>
@@ -1113,54 +1098,12 @@
     <t>Instrument Ids</t>
   </si>
   <si>
-    <t>2019-04-15T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-06-01T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-06-02T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-06-03T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-06-04T00:00:00.00Z</t>
-  </si>
-  <si>
     <t>Client</t>
   </si>
   <si>
-    <t>2019-04-16T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-04-17T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-04-18T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-04-19T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-04-20T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-04-21T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-04-22T00:00:00.00Z</t>
-  </si>
-  <si>
-    <t>2019-04-23T00:00:00.00Z</t>
-  </si>
-  <si>
     <t>Limit</t>
   </si>
   <si>
-    <t>Today in LUSID format</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -1182,7 +1125,40 @@
     <t>2028/12/01T00:00:00.00</t>
   </si>
   <si>
-    <t>2018/01/01T00:00:00.00</t>
+    <t>LUSID accepts datetimes in any recognised Excel format</t>
+  </si>
+  <si>
+    <t>LUSID also accepts UTC, UTS offsets and cutlabels</t>
+  </si>
+  <si>
+    <t>Excel formats to show datetime</t>
+  </si>
+  <si>
+    <t>Additional formats</t>
+  </si>
+  <si>
+    <t>Standard UTC timestamp:</t>
+  </si>
+  <si>
+    <t>Convert date into a string</t>
+  </si>
+  <si>
+    <t>UTC offset (not recognised as an excel date)</t>
+  </si>
+  <si>
+    <t>2019-04-10T13:30:45+04:00</t>
+  </si>
+  <si>
+    <t>Cutlabel</t>
+  </si>
+  <si>
+    <t>Add an hour to your datetime</t>
+  </si>
+  <si>
+    <t>Subtract a minute from your datetime</t>
+  </si>
+  <si>
+    <t>Excel</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1478,6 +1454,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1506,355 +1486,345 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
+    <main first="rtdsrv.c1066394fe78402db742926738641108">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>9df00e5b-0aca-4816-89e2-b83c524a13fe</stp>
-        <tr r="H30" s="10"/>
-        <tr r="F31" s="10"/>
-        <tr r="K26" s="10"/>
-        <tr r="I29" s="10"/>
-        <tr r="F28" s="10"/>
-        <tr r="K31" s="10"/>
-        <tr r="F25" s="10"/>
-        <tr r="G25" s="10"/>
-        <tr r="H24" s="10"/>
-        <tr r="K22" s="10"/>
-        <tr r="G30" s="10"/>
-        <tr r="I22" s="10"/>
-        <tr r="J27" s="10"/>
-        <tr r="I21" s="10"/>
-        <tr r="H27" s="10"/>
-        <tr r="F26" s="10"/>
-        <tr r="K24" s="10"/>
-        <tr r="F24" s="10"/>
-        <tr r="H23" s="10"/>
-        <tr r="I25" s="10"/>
-        <tr r="I27" s="10"/>
-        <tr r="G27" s="10"/>
-        <tr r="F30" s="10"/>
-        <tr r="J23" s="10"/>
-        <tr r="K27" s="10"/>
-        <tr r="I26" s="10"/>
-        <tr r="J30" s="10"/>
-        <tr r="G21" s="10"/>
-        <tr r="K23" s="10"/>
-        <tr r="I23" s="10"/>
-        <tr r="F27" s="10"/>
-        <tr r="I30" s="10"/>
-        <tr r="G28" s="10"/>
-        <tr r="G31" s="10"/>
-        <tr r="G26" s="10"/>
-        <tr r="G22" s="10"/>
-        <tr r="F22" s="10"/>
-        <tr r="J26" s="10"/>
-        <tr r="I31" s="10"/>
-        <tr r="J28" s="10"/>
-        <tr r="G23" s="10"/>
-        <tr r="K21" s="10"/>
-        <tr r="J29" s="10"/>
-        <tr r="K25" s="10"/>
-        <tr r="G29" s="10"/>
-        <tr r="H26" s="10"/>
-        <tr r="F23" s="10"/>
-        <tr r="J21" s="10"/>
-        <tr r="I28" s="10"/>
-        <tr r="J25" s="10"/>
-        <tr r="K28" s="10"/>
-        <tr r="K30" s="10"/>
-        <tr r="J22" s="10"/>
-        <tr r="J31" s="10"/>
-        <tr r="H21" s="10"/>
-        <tr r="K29" s="10"/>
-        <tr r="H29" s="10"/>
-        <tr r="G24" s="10"/>
-        <tr r="F29" s="10"/>
-        <tr r="H28" s="10"/>
-        <tr r="H31" s="10"/>
-        <tr r="J24" s="10"/>
-        <tr r="H25" s="10"/>
-        <tr r="I24" s="10"/>
-        <tr r="H22" s="10"/>
-        <tr r="F21" s="10"/>
-      </tp>
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>c67b2fbc-8155-48e2-95a0-1483d1438fc5</stp>
-        <tr r="M23" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>59b04c2c-3674-44eb-9460-801b75581a13</stp>
-        <tr r="E27" s="11"/>
-        <tr r="F17" s="11"/>
-        <tr r="E28" s="11"/>
-        <tr r="G23" s="11"/>
-        <tr r="G25" s="11"/>
-        <tr r="E26" s="11"/>
-        <tr r="G29" s="11"/>
-        <tr r="G17" s="11"/>
-        <tr r="G27" s="11"/>
-        <tr r="F25" s="11"/>
-        <tr r="E18" s="11"/>
-        <tr r="E22" s="11"/>
-        <tr r="F19" s="11"/>
-        <tr r="G22" s="11"/>
-        <tr r="E29" s="11"/>
-        <tr r="E21" s="11"/>
-        <tr r="F22" s="11"/>
-        <tr r="E20" s="11"/>
-        <tr r="F27" s="11"/>
-        <tr r="F26" s="11"/>
-        <tr r="F18" s="11"/>
-        <tr r="G19" s="11"/>
-        <tr r="E19" s="11"/>
-        <tr r="G26" s="11"/>
-        <tr r="E17" s="11"/>
-        <tr r="F29" s="11"/>
-        <tr r="E24" s="11"/>
-        <tr r="E23" s="11"/>
-        <tr r="F24" s="11"/>
-        <tr r="G24" s="11"/>
-        <tr r="F23" s="11"/>
-        <tr r="G20" s="11"/>
-        <tr r="F28" s="11"/>
-        <tr r="G28" s="11"/>
-        <tr r="E25" s="11"/>
-        <tr r="G18" s="11"/>
-        <tr r="F21" s="11"/>
-        <tr r="F20" s="11"/>
-        <tr r="G21" s="11"/>
-      </tp>
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>ba3b17ea-cafc-4caf-8423-75c21870757a</stp>
-        <tr r="M29" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>e1dfaffd-4d2f-4870-8544-0aa4fefc21af</stp>
-        <tr r="M26" s="16"/>
-      </tp>
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>eceaafb3-4b16-48c0-92c3-32e0375d8435</stp>
-        <tr r="M26" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>64f37c6d-7fb6-4ceb-8cee-04f66a5bfc26</stp>
+        <stp>5d0f56f9-f4c2-4c5a-94a9-2d1f0b6d93d4</stp>
         <tr r="M24" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>371c4718-3781-4230-a86a-f7142cb860fa</stp>
+        <stp>1183e152-0db1-44a2-a5d6-a18c0f443034</stp>
+        <tr r="M27" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c1066394fe78402db742926738641108">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>bef7f0fe-e638-4d05-a926-ffe23b5d107a</stp>
+        <tr r="M31" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c1066394fe78402db742926738641108">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>640283b9-62e1-4a6d-8b5d-d69ea050db43</stp>
         <tr r="M28" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>5949f5a1-47bb-4563-ac17-2f7518b7e33f</stp>
-        <tr r="M24" s="16"/>
+        <stp>2526ca4f-0263-477c-9521-5b5773a5caba</stp>
+        <tr r="I29" s="14"/>
+        <tr r="K29" s="14"/>
+        <tr r="F28" s="14"/>
+        <tr r="G29" s="14"/>
+        <tr r="F29" s="14"/>
+        <tr r="I28" s="14"/>
+        <tr r="F30" s="14"/>
+        <tr r="I30" s="14"/>
+        <tr r="J30" s="14"/>
+        <tr r="H30" s="14"/>
+        <tr r="H28" s="14"/>
+        <tr r="J28" s="14"/>
+        <tr r="J29" s="14"/>
+        <tr r="G30" s="14"/>
+        <tr r="K30" s="14"/>
+        <tr r="K28" s="14"/>
+        <tr r="H29" s="14"/>
+        <tr r="G28" s="14"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>9b07bf40-58c8-4721-98d7-82ef446c755e</stp>
-        <tr r="M25" s="16"/>
+        <stp>af95614e-0f89-4823-9402-5d9724906193</stp>
+        <tr r="N27" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c1066394fe78402db742926738641108">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>4e51a5a6-a497-4888-aa07-44dea3f77633</stp>
+        <tr r="M23" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>2b3ca304-ec44-4af6-a014-a27b7547fc52</stp>
-        <tr r="M27" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>01af2686-ec2f-4587-a098-a8fe103e0052</stp>
-        <tr r="M27" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>730166ca-0720-4fa2-a2d3-b5908ed41903</stp>
-        <tr r="M25" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>5ed556f8-69cb-453b-9233-b9edf4ef33e7</stp>
-        <tr r="G29" s="14"/>
-        <tr r="K28" s="14"/>
-        <tr r="J28" s="14"/>
-        <tr r="H29" s="14"/>
-        <tr r="K30" s="14"/>
-        <tr r="I30" s="14"/>
-        <tr r="K29" s="14"/>
-        <tr r="I28" s="14"/>
-        <tr r="J29" s="14"/>
-        <tr r="J30" s="14"/>
-        <tr r="F28" s="14"/>
-        <tr r="F29" s="14"/>
-        <tr r="G30" s="14"/>
-        <tr r="H30" s="14"/>
-        <tr r="F30" s="14"/>
-        <tr r="H28" s="14"/>
-        <tr r="I29" s="14"/>
-        <tr r="G28" s="14"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>d9e2f73a-c2fe-4ad1-88d9-480d02289923</stp>
-        <tr r="J34" s="13"/>
-        <tr r="G34" s="13"/>
-        <tr r="I35" s="13"/>
-        <tr r="F34" s="13"/>
-        <tr r="K36" s="13"/>
-        <tr r="J36" s="13"/>
-        <tr r="H35" s="13"/>
-        <tr r="I34" s="13"/>
-        <tr r="F35" s="13"/>
-        <tr r="J35" s="13"/>
-        <tr r="K34" s="13"/>
-        <tr r="H36" s="13"/>
-        <tr r="K35" s="13"/>
-        <tr r="G35" s="13"/>
-        <tr r="I36" s="13"/>
-        <tr r="H34" s="13"/>
-        <tr r="F36" s="13"/>
-        <tr r="G36" s="13"/>
+        <stp>aa39ede4-dfc6-45d3-9eff-6d5cf8a2baeb</stp>
+        <tr r="N25" s="16"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>bcb83465-0021-4ece-ba2f-0a7f0a955823</stp>
-        <tr r="M29" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>a8c86e4f-7bb8-46e7-b13c-6bb887f1d603</stp>
-        <tr r="M31" s="17"/>
+        <stp>2fc6ccee-f557-489b-9057-b3af262e3af2</stp>
+        <tr r="E29" s="11"/>
+        <tr r="G22" s="11"/>
+        <tr r="F28" s="11"/>
+        <tr r="E26" s="11"/>
+        <tr r="G20" s="11"/>
+        <tr r="G24" s="11"/>
+        <tr r="E19" s="11"/>
+        <tr r="F18" s="11"/>
+        <tr r="F21" s="11"/>
+        <tr r="F26" s="11"/>
+        <tr r="G23" s="11"/>
+        <tr r="G17" s="11"/>
+        <tr r="E22" s="11"/>
+        <tr r="G29" s="11"/>
+        <tr r="F29" s="11"/>
+        <tr r="F23" s="11"/>
+        <tr r="E24" s="11"/>
+        <tr r="F27" s="11"/>
+        <tr r="E28" s="11"/>
+        <tr r="F17" s="11"/>
+        <tr r="E18" s="11"/>
+        <tr r="G28" s="11"/>
+        <tr r="E25" s="11"/>
+        <tr r="G18" s="11"/>
+        <tr r="G21" s="11"/>
+        <tr r="G26" s="11"/>
+        <tr r="E23" s="11"/>
+        <tr r="E20" s="11"/>
+        <tr r="F19" s="11"/>
+        <tr r="F25" s="11"/>
+        <tr r="F22" s="11"/>
+        <tr r="F20" s="11"/>
+        <tr r="E27" s="11"/>
+        <tr r="E21" s="11"/>
+        <tr r="G27" s="11"/>
+        <tr r="E17" s="11"/>
+        <tr r="F24" s="11"/>
+        <tr r="G19" s="11"/>
+        <tr r="G25" s="11"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>b4b3d1ba-cf6a-4fff-8fb9-dc3977dcc43a</stp>
-        <tr r="M30" s="16"/>
+        <stp>45bb2e96-88fc-40c9-b440-49dbe9bdc57a</stp>
+        <tr r="F35" s="13"/>
+        <tr r="I36" s="13"/>
+        <tr r="G34" s="13"/>
+        <tr r="I35" s="13"/>
+        <tr r="H35" s="13"/>
+        <tr r="H34" s="13"/>
+        <tr r="G36" s="13"/>
+        <tr r="F36" s="13"/>
+        <tr r="G35" s="13"/>
+        <tr r="J34" s="13"/>
+        <tr r="H36" s="13"/>
+        <tr r="F34" s="13"/>
+        <tr r="K34" s="13"/>
+        <tr r="J35" s="13"/>
+        <tr r="K35" s="13"/>
+        <tr r="I34" s="13"/>
+        <tr r="J36" s="13"/>
+        <tr r="K36" s="13"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c1066394fe78402db742926738641108">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>8f1191bb-f2f7-49b0-b69f-2e5f48e396fe</stp>
+        <tr r="M29" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>7b07e525-fa58-44cc-897a-8230168adc94</stp>
-        <tr r="G40" s="20"/>
-        <tr r="H39" s="20"/>
-        <tr r="G39" s="20"/>
-        <tr r="F39" s="20"/>
-        <tr r="I40" s="20"/>
-        <tr r="K39" s="20"/>
-        <tr r="L40" s="20"/>
-        <tr r="K40" s="20"/>
-        <tr r="J39" s="20"/>
-        <tr r="J40" s="20"/>
-        <tr r="H40" s="20"/>
-        <tr r="L39" s="20"/>
-        <tr r="I39" s="20"/>
-        <tr r="F40" s="20"/>
+        <stp>895f9df5-8a61-47b6-8d68-fecf2dee3704</stp>
+        <tr r="N26" s="16"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>a267f150-b8dc-4b11-b67c-ee26e6fe2754</stp>
-        <tr r="M28" s="16"/>
+        <stp>cbe24929-60f5-416a-ae87-b19f15f26d9c</stp>
+        <tr r="M25" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>96093ff9-abbb-4205-99e9-e162126b8a8d</stp>
-        <tr r="M23" s="16"/>
+        <stp>d51e9e18-460f-4650-8668-982376bb58d4</stp>
+        <tr r="G21" s="10"/>
+        <tr r="H21" s="10"/>
+        <tr r="I30" s="10"/>
+        <tr r="I31" s="10"/>
+        <tr r="K23" s="10"/>
+        <tr r="G28" s="10"/>
+        <tr r="K28" s="10"/>
+        <tr r="J25" s="10"/>
+        <tr r="G23" s="10"/>
+        <tr r="K22" s="10"/>
+        <tr r="F23" s="10"/>
+        <tr r="J22" s="10"/>
+        <tr r="G31" s="10"/>
+        <tr r="J28" s="10"/>
+        <tr r="H26" s="10"/>
+        <tr r="J26" s="10"/>
+        <tr r="K26" s="10"/>
+        <tr r="H27" s="10"/>
+        <tr r="K30" s="10"/>
+        <tr r="H29" s="10"/>
+        <tr r="H23" s="10"/>
+        <tr r="F21" s="10"/>
+        <tr r="I21" s="10"/>
+        <tr r="I24" s="10"/>
+        <tr r="I29" s="10"/>
+        <tr r="F30" s="10"/>
+        <tr r="I23" s="10"/>
+        <tr r="J30" s="10"/>
+        <tr r="I25" s="10"/>
+        <tr r="I22" s="10"/>
+        <tr r="H22" s="10"/>
+        <tr r="K29" s="10"/>
+        <tr r="H30" s="10"/>
+        <tr r="F24" s="10"/>
+        <tr r="I26" s="10"/>
+        <tr r="J23" s="10"/>
+        <tr r="F29" s="10"/>
+        <tr r="G25" s="10"/>
+        <tr r="K25" s="10"/>
+        <tr r="K27" s="10"/>
+        <tr r="H28" s="10"/>
+        <tr r="I28" s="10"/>
+        <tr r="G26" s="10"/>
+        <tr r="K31" s="10"/>
+        <tr r="J24" s="10"/>
+        <tr r="H31" s="10"/>
+        <tr r="H24" s="10"/>
+        <tr r="I27" s="10"/>
+        <tr r="K21" s="10"/>
+        <tr r="G29" s="10"/>
+        <tr r="J31" s="10"/>
+        <tr r="G30" s="10"/>
+        <tr r="K24" s="10"/>
+        <tr r="F31" s="10"/>
+        <tr r="J27" s="10"/>
+        <tr r="G24" s="10"/>
+        <tr r="F28" s="10"/>
+        <tr r="F22" s="10"/>
+        <tr r="F26" s="10"/>
+        <tr r="G22" s="10"/>
+        <tr r="F27" s="10"/>
+        <tr r="J21" s="10"/>
+        <tr r="J29" s="10"/>
+        <tr r="F25" s="10"/>
+        <tr r="G27" s="10"/>
+        <tr r="H25" s="10"/>
       </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>3e309b10-765b-4cf5-9954-c0558606d071</stp>
-        <tr r="M22" s="16"/>
-        <tr r="M22" s="17"/>
+        <stp>4228cb2a-3307-4856-90cc-d4503b20a467</stp>
+        <tr r="M30" s="17"/>
       </tp>
-    </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>7e2b769e-a7f0-4dde-b4d9-0a0d7eb5d124</stp>
-        <tr r="M30" s="17"/>
+        <stp>a4edf342-50f5-4eef-aa2f-331fa2f8b221</stp>
+        <tr r="M22" s="17"/>
+        <tr r="N22" s="16"/>
       </tp>
     </main>
-    <main first="rtdsrv.a451133d7b174878998c0bed4b7b8852">
+    <main first="rtdsrv.c1066394fe78402db742926738641108">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>07ff1651-663d-41ce-a831-61ef56dd9b2f</stp>
-        <tr r="G33" s="12"/>
+        <stp>05f639ab-f941-49ea-9358-2e11e38b4054</stp>
+        <tr r="M26" s="17"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>1f6956f5-70ba-40c5-a2b8-95d9c9b5bdf3</stp>
+        <tr r="N28" s="16"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>be9da83e-258a-464f-bd50-93ef7b47b59d</stp>
+        <tr r="N29" s="16"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>684c7864-9e83-4d46-ad0b-56bc6c06a3f3</stp>
+        <tr r="N30" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c1066394fe78402db742926738641108">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>990b63ef-1cdf-4a9f-ba60-4b34a2d1ba94</stp>
+        <tr r="N24" s="16"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>a1d2269c-2c6b-4a07-898a-ce1ed317e62b</stp>
+        <tr r="E30" s="12"/>
+        <tr r="G28" s="12"/>
+        <tr r="G23" s="12"/>
+        <tr r="G24" s="12"/>
+        <tr r="F32" s="12"/>
         <tr r="F33" s="12"/>
-        <tr r="E33" s="12"/>
+        <tr r="F23" s="12"/>
+        <tr r="G26" s="12"/>
+        <tr r="E31" s="12"/>
         <tr r="G32" s="12"/>
-        <tr r="F32" s="12"/>
-        <tr r="E32" s="12"/>
-        <tr r="G31" s="12"/>
-        <tr r="F31" s="12"/>
-        <tr r="E31" s="12"/>
-        <tr r="G30" s="12"/>
-        <tr r="F30" s="12"/>
-        <tr r="E30" s="12"/>
-        <tr r="G29" s="12"/>
-        <tr r="F29" s="12"/>
-        <tr r="E29" s="12"/>
-        <tr r="G28" s="12"/>
-        <tr r="F28" s="12"/>
-        <tr r="E28" s="12"/>
-        <tr r="G27" s="12"/>
-        <tr r="F27" s="12"/>
-        <tr r="E27" s="12"/>
-        <tr r="G26" s="12"/>
-        <tr r="F26" s="12"/>
-        <tr r="E26" s="12"/>
-        <tr r="G25" s="12"/>
-        <tr r="F25" s="12"/>
-        <tr r="E25" s="12"/>
-        <tr r="G24" s="12"/>
         <tr r="F24" s="12"/>
         <tr r="E24" s="12"/>
-        <tr r="G23" s="12"/>
-        <tr r="F23" s="12"/>
+        <tr r="G31" s="12"/>
+        <tr r="E28" s="12"/>
+        <tr r="E25" s="12"/>
+        <tr r="F31" s="12"/>
+        <tr r="E27" s="12"/>
+        <tr r="E32" s="12"/>
+        <tr r="F27" s="12"/>
+        <tr r="G25" s="12"/>
         <tr r="E23" s="12"/>
+        <tr r="F26" s="12"/>
+        <tr r="E33" s="12"/>
+        <tr r="E26" s="12"/>
+        <tr r="G33" s="12"/>
+        <tr r="F30" s="12"/>
+        <tr r="F29" s="12"/>
+        <tr r="G27" s="12"/>
+        <tr r="G29" s="12"/>
+        <tr r="G30" s="12"/>
+        <tr r="F25" s="12"/>
+        <tr r="F28" s="12"/>
+        <tr r="E29" s="12"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>2abd65be-3451-48d8-80c7-8ba41241f749</stp>
+        <tr r="N23" s="16"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>793d53bd-4596-4c68-a3a0-c593d641885a</stp>
+        <tr r="I39" s="20"/>
+        <tr r="F40" s="20"/>
+        <tr r="I40" s="20"/>
+        <tr r="J39" s="20"/>
+        <tr r="H39" s="20"/>
+        <tr r="F39" s="20"/>
+        <tr r="J40" s="20"/>
+        <tr r="H40" s="20"/>
+        <tr r="L40" s="20"/>
+        <tr r="K40" s="20"/>
+        <tr r="G39" s="20"/>
+        <tr r="G40" s="20"/>
+        <tr r="K39" s="20"/>
+        <tr r="L39" s="20"/>
       </tp>
     </main>
   </volType>
@@ -1881,7 +1851,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2ED52D2-A341-4FDD-B366-B7D02A283EE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C85DD34-7D92-485A-8C32-1AA5D0B93616}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1904,7 +1874,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="17866099" y="324971"/>
+          <a:off x="17894674" y="324971"/>
           <a:ext cx="2122396" cy="1277309"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2465,8 +2435,8 @@
       <xdr:rowOff>33619</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>235325</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190502</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>96210</xdr:rowOff>
     </xdr:to>
@@ -2599,8 +2569,8 @@
       <sheetName val="View Transactions"/>
       <sheetName val="Perform a reconciliation"/>
       <sheetName val="Upload Transactions"/>
+      <sheetName val="Set Holdings"/>
       <sheetName val="Create Portfolio"/>
-      <sheetName val="Set Holdings"/>
       <sheetName val="Inputs"/>
     </sheetNames>
     <sheetDataSet>
@@ -2916,14 +2886,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE2DA83-ACF2-4349-84B3-AF9C1F47D679}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94E7776-639F-42A4-B6AA-8D3309A3EB23}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:T26"/>
+  <dimension ref="B1:T31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:J24"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,8 +2905,8 @@
     <col min="5" max="5" width="50.42578125" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" style="23" customWidth="1"/>
     <col min="7" max="7" width="22" style="23" customWidth="1"/>
-    <col min="8" max="8" width="43.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" style="23" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" style="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" style="23" customWidth="1"/>
     <col min="11" max="11" width="22" style="23" customWidth="1"/>
     <col min="12" max="14" width="24.28515625" style="23" customWidth="1"/>
@@ -3110,10 +3080,14 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>321</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>322</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -3126,14 +3100,10 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="9" t="s">
-        <v>258</v>
-      </c>
+      <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>259</v>
-      </c>
+      <c r="H14" s="9"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -3142,14 +3112,18 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="E15" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>324</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -3159,26 +3133,16 @@
       <c r="O15" s="2"/>
       <c r="T15" s="27"/>
     </row>
-    <row r="16" spans="2:20" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F16" s="25">
-        <v>43565</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>314</v>
-      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -3186,16 +3150,26 @@
       <c r="O16" s="2"/>
       <c r="T16" s="27"/>
     </row>
-    <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F17" s="25">
+        <v>43565</v>
+      </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>309</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -3207,21 +3181,11 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="F18" s="28">
-        <f>F16</f>
-        <v>43565</v>
-      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="I18" s="25" t="str">
-        <f>TEXT(F16,"yyyy-mm-dd")&amp;"T"&amp;TEXT(F16,"hh:mm:ss.00Z")</f>
-        <v>2019-04-10T00:00:00.00Z</v>
-      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -3234,11 +3198,21 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F19" s="28">
+        <f>F17</f>
+        <v>43565</v>
+      </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I19" s="25" t="str">
+        <f>TEXT(F23,"yyyy-mm-dd")&amp;"T"&amp;TEXT(F23," hh:mm:ss.00Z")</f>
+        <v>2019-04-10T 13:30:45.55Z</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -3247,24 +3221,15 @@
       <c r="O19" s="2"/>
       <c r="T19" s="27"/>
     </row>
-    <row r="20" spans="2:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F20" s="29">
-        <v>0.56302719907407406</v>
-      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="I20" s="25" t="str">
-        <f>TEXT(F18,"yyyy-mm-dd")&amp;"T"&amp;TEXT(F18,"hh:mm:ss.00Z")</f>
-        <v>2019-04-10T00:00:00.00Z</v>
-      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -3277,12 +3242,20 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F21" s="29">
+        <v>0.56302719907407406</v>
+      </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="J21" s="51"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -3294,37 +3267,38 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F22" s="30">
-        <f>F16 + F20</f>
-        <v>43565.563027199074</v>
-      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="I22" s="25" t="str">
-        <f>TEXT(F22,"yyyy-mm-dd")&amp;"T"&amp;TEXT(F22,"hh:mm:ss.00Z")</f>
-        <v>2019-04-10T13:30:45.55Z</v>
-      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
+      <c r="T22" s="27"/>
     </row>
     <row r="23" spans="2:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F23" s="30">
+        <f>F17 + F21</f>
+        <v>43565.563027199074</v>
+      </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I23" s="25" t="str">
+        <f>TEXT(F23,"yyyy-mm-dd")&amp;"NSingaporeClose"</f>
+        <v>2019-04-10NSingaporeClose</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -3336,21 +3310,11 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F24" s="31">
-        <f>F22</f>
-        <v>43565.563027199074</v>
-      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="I24" s="25" t="str">
-        <f ca="1">TEXT(NOW(),"yyyy-mm-dd")&amp;"T"&amp;TEXT(NOW(),"hh:mm:ss.00Z")</f>
-        <v>2019-08-20T15:01:44.10Z</v>
-      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -3358,12 +3322,17 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F25" s="31">
+        <f>F23</f>
+        <v>43565.563027199074</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -3374,7 +3343,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="2:20" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3390,11 +3359,101 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
     </row>
+    <row r="27" spans="2:20" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F27" s="30">
+        <f>F23+1/24</f>
+        <v>43565.604693865738</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F29" s="30">
+        <f>F27-1/1440</f>
+        <v>43565.603999421292</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" xr:uid="{CF85FD4A-F7A8-4952-BA30-59D23A483846}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{20ADEA89-BDA9-475C-850D-FE4616934C3E}"/>
-    <hyperlink ref="E9" r:id="rId3" xr:uid="{3B31D428-C70D-4A25-ADA8-BB79AD0C4650}"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{04DB46FB-6D1A-463C-9BFC-4C724D357CC3}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{08DD694B-05A4-451E-93AA-55AB189623A1}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{7B4C5A5A-871F-47CA-B31D-9ED042440010}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -3410,7 +3469,7 @@
   <dimension ref="A1:AD55"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3459,7 +3518,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3497,7 +3556,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3705,7 +3764,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -3811,7 +3870,7 @@
     <row r="19" spans="2:30" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="10" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -3922,7 +3981,7 @@
         <v>208</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>209</v>
@@ -3940,16 +3999,16 @@
         <v>185</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>227</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22"/>
@@ -3973,7 +4032,9 @@
       <c r="E23" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="18" t="s">
+        <v>332</v>
+      </c>
       <c r="G23" s="13" t="s">
         <v>204</v>
       </c>
@@ -3992,14 +4053,14 @@
       <c r="L23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="M23" s="20" t="s">
-        <v>317</v>
+      <c r="M23" s="20">
+        <v>43570</v>
       </c>
       <c r="N23" s="48"/>
       <c r="O23" s="32"/>
       <c r="P23" s="32" t="str">
         <f>_xll.flQuotesAdd(F15,E22:O23)</f>
-        <v>Added 1 quote(s) as at time 2019-08-20 13:22:03Z</v>
+        <v>Added 1 quote(s) as at time 2019-09-03 16:02:48Z</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23"/>
@@ -4679,7 +4740,7 @@
   <dimension ref="B1:Y43"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4726,7 +4787,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4764,7 +4825,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4966,7 +5027,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -5065,7 +5126,7 @@
     <row r="19" spans="2:25" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="10" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -5113,7 +5174,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -5181,7 +5242,7 @@
         <v>208</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>209</v>
@@ -5199,16 +5260,16 @@
         <v>185</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="N23" s="6" t="s">
         <v>227</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23"/>
@@ -5225,10 +5286,10 @@
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="13" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>215</v>
@@ -5248,14 +5309,14 @@
       <c r="L24" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="M24" s="20" t="s">
-        <v>318</v>
+      <c r="M24" s="20">
+        <v>43617</v>
       </c>
       <c r="N24" s="32"/>
       <c r="O24" s="32"/>
       <c r="P24" s="32" t="str">
         <f>_xll.flQuotesAdd(F15,E23:O27)</f>
-        <v>Added 4 quote(s) as at time 2019-08-20 13:22:03Z</v>
+        <v>Added 4 quote(s) as at time 2019-09-03 16:02:48Z</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24"/>
@@ -5272,10 +5333,10 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
       <c r="E25" s="13" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>215</v>
@@ -5295,8 +5356,9 @@
       <c r="L25" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="M25" s="20" t="s">
-        <v>319</v>
+      <c r="M25" s="20">
+        <f>M24+1</f>
+        <v>43618</v>
       </c>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
@@ -5316,10 +5378,10 @@
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
       <c r="E26" s="13" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>215</v>
@@ -5339,8 +5401,9 @@
       <c r="L26" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="M26" s="20" t="s">
-        <v>320</v>
+      <c r="M26" s="20">
+        <f t="shared" ref="M26:M27" si="0">M25+1</f>
+        <v>43619</v>
       </c>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
@@ -5360,10 +5423,10 @@
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
       <c r="E27" s="13" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>215</v>
@@ -5383,8 +5446,9 @@
       <c r="L27" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="M27" s="20" t="s">
-        <v>321</v>
+      <c r="M27" s="20">
+        <f t="shared" si="0"/>
+        <v>43620</v>
       </c>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
@@ -6564,7 +6628,7 @@
   <dimension ref="B1:R30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6755,7 +6819,7 @@
     <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -6816,13 +6880,13 @@
       <c r="D17" s="2"/>
       <c r="E17" s="33" t="str">
         <f t="array" ref="E17:G29">_xll.flInstrumentTypesGet()</f>
-        <v>[More...]</v>
+        <v>IdentifierType</v>
       </c>
       <c r="F17" s="33" t="str">
-        <v>[More...]</v>
+        <v>PropertyKey</v>
       </c>
       <c r="G17" s="33" t="str">
-        <v>[More...]</v>
+        <v>IsUniqueIdentifierType</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -6838,13 +6902,13 @@
       <c r="C18" s="2"/>
       <c r="D18" s="9"/>
       <c r="E18" s="18" t="str">
-        <v>[More...]</v>
+        <v>LusidInstrumentId</v>
       </c>
       <c r="F18" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G18" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/LusidInstrumentId</v>
+      </c>
+      <c r="G18" s="18" t="b">
+        <v>1</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -6860,13 +6924,13 @@
       <c r="C19" s="2"/>
       <c r="D19" s="9"/>
       <c r="E19" s="37" t="str">
-        <v>[More...]</v>
+        <v>Figi</v>
       </c>
       <c r="F19" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G19" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/Figi</v>
+      </c>
+      <c r="G19" s="18" t="b">
+        <v>1</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -6882,13 +6946,13 @@
       <c r="C20" s="2"/>
       <c r="D20" s="9"/>
       <c r="E20" s="37" t="str">
-        <v>[More...]</v>
+        <v>RIC</v>
       </c>
       <c r="F20" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G20" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/RIC</v>
+      </c>
+      <c r="G20" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -6904,13 +6968,13 @@
       <c r="C21" s="2"/>
       <c r="D21" s="9"/>
       <c r="E21" s="37" t="str">
-        <v>[More...]</v>
+        <v>Cusip</v>
       </c>
       <c r="F21" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G21" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/Cusip</v>
+      </c>
+      <c r="G21" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -6926,13 +6990,13 @@
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
       <c r="E22" s="37" t="str">
-        <v>[More...]</v>
+        <v>Ticker</v>
       </c>
       <c r="F22" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G22" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/Ticker</v>
+      </c>
+      <c r="G22" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -6948,13 +7012,13 @@
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
       <c r="E23" s="37" t="str">
-        <v>[More...]</v>
+        <v>Isin</v>
       </c>
       <c r="F23" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G23" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/Isin</v>
+      </c>
+      <c r="G23" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -6970,13 +7034,13 @@
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="37" t="str">
-        <v>[More...]</v>
+        <v>Wertpapier</v>
       </c>
       <c r="F24" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G24" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/Wertpapier</v>
+      </c>
+      <c r="G24" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -6991,13 +7055,13 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
       <c r="E25" s="37" t="str">
-        <v>[More...]</v>
+        <v>QuotePermId</v>
       </c>
       <c r="F25" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G25" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/QuotePermId</v>
+      </c>
+      <c r="G25" s="18" t="b">
+        <v>1</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -7010,13 +7074,13 @@
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
       <c r="E26" s="37" t="str">
-        <v>[More...]</v>
+        <v>ShareClassFigi</v>
       </c>
       <c r="F26" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G26" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/ShareClassFigi</v>
+      </c>
+      <c r="G26" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -7029,13 +7093,13 @@
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
       <c r="E27" s="37" t="str">
-        <v>[More...]</v>
+        <v>CompositeFigi</v>
       </c>
       <c r="F27" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G27" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/CompositeFigi</v>
+      </c>
+      <c r="G27" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -7048,13 +7112,13 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="37" t="str">
-        <v>[More...]</v>
+        <v>ClientInternal</v>
       </c>
       <c r="F28" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G28" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/ClientInternal</v>
+      </c>
+      <c r="G28" s="18" t="b">
+        <v>1</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -7067,13 +7131,13 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="37" t="str">
-        <v>[More...]</v>
+        <v>Sedol</v>
       </c>
       <c r="F29" s="18" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G29" s="18" t="str">
-        <v>[More...]</v>
+        <v>Instrument/default/Sedol</v>
+      </c>
+      <c r="G29" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -7126,7 +7190,7 @@
   <dimension ref="B1:K34"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E23:E24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7288,7 +7352,7 @@
     <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
       <c r="C14" s="10" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -7376,7 +7440,7 @@
         <v>198</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -7387,13 +7451,12 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="25" t="str">
-        <f ca="1">TEXT(NOW(),"yyyy-mm-dd")&amp;"T"&amp;TEXT(NOW(),"hh:mm:ss.00Z")</f>
-        <v>2019-08-20T15:01:44.10Z</v>
-      </c>
-      <c r="F21" s="25" t="str">
-        <f ca="1">TEXT(NOW(),"yyyy-mm-dd")&amp;"T"&amp;TEXT(NOW(),"hh:mm:ss.00Z")</f>
-        <v>2019-08-20T15:01:44.10Z</v>
+      <c r="E21" s="25">
+        <f ca="1">NOW()</f>
+        <v>43711.710300231483</v>
+      </c>
+      <c r="F21" s="25">
+        <v>43697</v>
       </c>
       <c r="G21" s="49">
         <v>5</v>
@@ -7420,7 +7483,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="33" t="str">
-        <f t="array" aca="1" ref="E23:G33" ca="1">_xll.flInstrumentsGetAll(E21,F21,G21)</f>
+        <f t="array" ref="E23:G33" ca="1">_xll.flInstrumentsGetAll(E21,F21,G21)</f>
         <v>State</v>
       </c>
       <c r="F23" s="33" t="str">
@@ -7557,17 +7620,17 @@
       <c r="D29" s="2">
         <v>6</v>
       </c>
-      <c r="E29" s="37" t="str">
+      <c r="E29" s="37" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F29" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="F29" s="18" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G29" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="G29" s="18" t="e">
         <f ca="1"/>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -7580,17 +7643,17 @@
       <c r="D30" s="2">
         <v>7</v>
       </c>
-      <c r="E30" s="37" t="str">
+      <c r="E30" s="37" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F30" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="F30" s="18" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G30" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="G30" s="18" t="e">
         <f ca="1"/>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -7603,17 +7666,17 @@
       <c r="D31" s="2">
         <v>8</v>
       </c>
-      <c r="E31" s="37" t="str">
+      <c r="E31" s="37" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F31" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="F31" s="18" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G31" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="G31" s="18" t="e">
         <f ca="1"/>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -7626,17 +7689,17 @@
       <c r="D32" s="2">
         <v>9</v>
       </c>
-      <c r="E32" s="37" t="str">
+      <c r="E32" s="37" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F32" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="F32" s="18" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G32" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="G32" s="18" t="e">
         <f ca="1"/>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -7649,17 +7712,17 @@
       <c r="D33" s="2">
         <v>10</v>
       </c>
-      <c r="E33" s="37" t="str">
+      <c r="E33" s="37" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F33" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="F33" s="18" t="e">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G33" s="18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="G33" s="18" t="e">
         <f ca="1"/>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -7698,7 +7761,7 @@
   <dimension ref="B1:R32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7874,7 +7937,7 @@
     <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -7996,22 +8059,22 @@
       </c>
       <c r="F21" s="33" t="str">
         <f t="array" ref="F21:K31">_xll.flInstrumentsLookup(F19,E22:E31)</f>
-        <v>[More...]</v>
+        <v>State</v>
       </c>
       <c r="G21" s="33" t="str">
-        <v>[More...]</v>
+        <v>LusidInstrumentId</v>
       </c>
       <c r="H21" s="34" t="str">
-        <v>[More...]</v>
+        <v>Name</v>
       </c>
       <c r="I21" s="33" t="str">
-        <v>[More...]</v>
+        <v>Figi</v>
       </c>
       <c r="J21" s="33" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K21" s="33" t="str">
-        <v>[More...]</v>
+        <v>ClientInternal</v>
+      </c>
+      <c r="K21" s="33" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L21" s="2"/>
       <c r="P21" s="19"/>
@@ -8028,22 +8091,22 @@
         <v>188</v>
       </c>
       <c r="F22" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G22" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_RVXW0J4Z</v>
       </c>
       <c r="H22" s="35" t="str">
-        <v>[More...]</v>
+        <v>Apple</v>
       </c>
       <c r="I22" s="35" t="str">
-        <v>[More...]</v>
+        <v>BBG000B9XRY4</v>
       </c>
       <c r="J22" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K22" s="36" t="str">
-        <v>[More...]</v>
+        <v>ExcelID1</v>
+      </c>
+      <c r="K22" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L22" s="2"/>
       <c r="P22" s="19"/>
@@ -8060,22 +8123,22 @@
         <v>189</v>
       </c>
       <c r="F23" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G23" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_T2QB43BD</v>
       </c>
       <c r="H23" s="35" t="str">
-        <v>[More...]</v>
+        <v>JPMorgan Chase</v>
       </c>
       <c r="I23" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J23" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K23" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG000DMBXR2</v>
+      </c>
+      <c r="J23" s="36">
+        <v>0</v>
+      </c>
+      <c r="K23" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L23" s="2"/>
       <c r="P23" s="19"/>
@@ -8092,22 +8155,22 @@
         <v>190</v>
       </c>
       <c r="F24" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G24" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_XUE1ELEX</v>
       </c>
       <c r="H24" s="35" t="str">
-        <v>[More...]</v>
+        <v>BP</v>
       </c>
       <c r="I24" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J24" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K24" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG000C059M6</v>
+      </c>
+      <c r="J24" s="36">
+        <v>0</v>
+      </c>
+      <c r="K24" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L24" s="2"/>
       <c r="P24" s="19"/>
@@ -8124,22 +8187,22 @@
         <v>191</v>
       </c>
       <c r="F25" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G25" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_DDZQNCD6</v>
       </c>
       <c r="H25" s="35" t="str">
-        <v>[More...]</v>
+        <v>Anheuser-Busch InBev</v>
       </c>
       <c r="I25" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J25" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K25" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG00DQ4YZ36</v>
+      </c>
+      <c r="J25" s="36">
+        <v>0</v>
+      </c>
+      <c r="K25" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L25" s="2"/>
       <c r="P25" s="19"/>
@@ -8156,22 +8219,22 @@
         <v>192</v>
       </c>
       <c r="F26" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G26" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_BVE0REZ5</v>
       </c>
       <c r="H26" s="35" t="str">
-        <v>[More...]</v>
+        <v>Toyota Motor</v>
       </c>
       <c r="I26" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J26" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K26" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG000BCM915</v>
+      </c>
+      <c r="J26" s="36">
+        <v>0</v>
+      </c>
+      <c r="K26" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L26" s="2"/>
       <c r="P26" s="19"/>
@@ -8188,22 +8251,22 @@
         <v>193</v>
       </c>
       <c r="F27" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G27" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_UX4RG8N5</v>
       </c>
       <c r="H27" s="35" t="str">
-        <v>[More...]</v>
+        <v>Volkswagen</v>
       </c>
       <c r="I27" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J27" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K27" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG000BCH458</v>
+      </c>
+      <c r="J27" s="36">
+        <v>0</v>
+      </c>
+      <c r="K27" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L27" s="2"/>
       <c r="P27" s="19"/>
@@ -8220,22 +8283,22 @@
         <v>194</v>
       </c>
       <c r="F28" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G28" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_HP2NME8I</v>
       </c>
       <c r="H28" s="35" t="str">
-        <v>[More...]</v>
+        <v>HSBC Holdings</v>
       </c>
       <c r="I28" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J28" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K28" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG000BS1MT4</v>
+      </c>
+      <c r="J28" s="36">
+        <v>0</v>
+      </c>
+      <c r="K28" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L28" s="2"/>
       <c r="Q28" s="19"/>
@@ -8251,22 +8314,22 @@
         <v>195</v>
       </c>
       <c r="F29" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G29" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_9SBVLHHA</v>
       </c>
       <c r="H29" s="35" t="str">
-        <v>[More...]</v>
+        <v>Walt Disney</v>
       </c>
       <c r="I29" s="35" t="str">
-        <v>[More...]</v>
+        <v>BBG000BH4R78</v>
       </c>
       <c r="J29" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K29" s="36" t="str">
-        <v>[More...]</v>
+        <v>ExcelID22</v>
+      </c>
+      <c r="K29" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L29" s="2"/>
     </row>
@@ -8280,22 +8343,22 @@
         <v>196</v>
       </c>
       <c r="F30" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G30" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_JFJASSYO</v>
       </c>
       <c r="H30" s="35" t="str">
-        <v>[More...]</v>
+        <v>Microsoft</v>
       </c>
       <c r="I30" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J30" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K30" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG000BPH459</v>
+      </c>
+      <c r="J30" s="36">
+        <v>0</v>
+      </c>
+      <c r="K30" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L30" s="2"/>
     </row>
@@ -8309,22 +8372,22 @@
         <v>197</v>
       </c>
       <c r="F31" s="18" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G31" s="18" t="str">
-        <v>[More...]</v>
+        <v>LUID_0UK37N0H</v>
       </c>
       <c r="H31" s="35" t="str">
-        <v>[More...]</v>
+        <v>Softbank</v>
       </c>
       <c r="I31" s="35" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J31" s="36" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K31" s="36" t="str">
-        <v>[More...]</v>
+        <v>BBG000CLY2D3</v>
+      </c>
+      <c r="J31" s="36">
+        <v>0</v>
+      </c>
+      <c r="K31" s="36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L31" s="2"/>
     </row>
@@ -8373,7 +8436,7 @@
   <dimension ref="B1:S48"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:H15"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8619,7 +8682,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -8652,22 +8715,22 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="8" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>218</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="K18" s="8"/>
       <c r="L18" s="2"/>
@@ -8692,22 +8755,22 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="8" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>218</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>221</v>
@@ -8730,7 +8793,7 @@
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="17" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15" t="str">
@@ -8759,22 +8822,22 @@
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>218</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>221</v>
@@ -8797,7 +8860,7 @@
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="17" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15" t="str">
@@ -8936,22 +8999,22 @@
       </c>
       <c r="F34" s="8" t="str">
         <f t="array" ref="F34:K36">_xll.flInstrumentsLookup(F32,E35:E36)</f>
-        <v>[More...]</v>
+        <v>State</v>
       </c>
       <c r="G34" s="8" t="str">
-        <v>[More...]</v>
+        <v>LusidInstrumentId</v>
       </c>
       <c r="H34" s="7" t="str">
-        <v>[More...]</v>
+        <v>Name</v>
       </c>
       <c r="I34" s="8" t="str">
-        <v>[More...]</v>
+        <v>Figi</v>
       </c>
       <c r="J34" s="8" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K34" s="8" t="str">
-        <v>[More...]</v>
+        <v>ClientInternal</v>
+      </c>
+      <c r="K34" s="8" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
@@ -8965,22 +9028,22 @@
         <v>BBG000B9XRY4</v>
       </c>
       <c r="F35" s="13" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G35" s="13" t="str">
-        <v>[More...]</v>
+        <v>LUID_RVXW0J4Z</v>
       </c>
       <c r="H35" s="16" t="str">
-        <v>[More...]</v>
+        <v>Apple</v>
       </c>
       <c r="I35" s="16" t="str">
-        <v>[More...]</v>
+        <v>BBG000B9XRY4</v>
       </c>
       <c r="J35" s="17" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K35" s="17" t="str">
-        <v>[More...]</v>
+        <v>ExcelID1</v>
+      </c>
+      <c r="K35" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -8994,22 +9057,22 @@
         <v>BBG000BH4R78</v>
       </c>
       <c r="F36" s="13" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G36" s="13" t="str">
-        <v>[More...]</v>
+        <v>LUID_9SBVLHHA</v>
       </c>
       <c r="H36" s="16" t="str">
-        <v>[More...]</v>
+        <v>Walt Disney</v>
       </c>
       <c r="I36" s="16" t="str">
-        <v>[More...]</v>
+        <v>BBG000BH4R78</v>
       </c>
       <c r="J36" s="17" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K36" s="17" t="str">
-        <v>[More...]</v>
+        <v>ExcelID22</v>
+      </c>
+      <c r="K36" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -9219,7 +9282,7 @@
   <dimension ref="B1:M31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9265,7 +9328,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -9295,7 +9358,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -9480,22 +9543,22 @@
       <c r="C18" s="2"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>218</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>221</v>
@@ -9641,22 +9704,22 @@
       </c>
       <c r="F28" s="8" t="str">
         <f t="array" ref="F28:K30">_xll.flInstrumentsLookup(F26,E29,"Instrument/default/Ticker")</f>
-        <v>[More...]</v>
+        <v>State</v>
       </c>
       <c r="G28" s="8" t="str">
-        <v>[More...]</v>
+        <v>LusidInstrumentId</v>
       </c>
       <c r="H28" s="7" t="str">
-        <v>[More...]</v>
+        <v>Name</v>
       </c>
       <c r="I28" s="8" t="str">
-        <v>[More...]</v>
+        <v>Ticker</v>
       </c>
       <c r="J28" s="8" t="str">
-        <v>[More...]</v>
+        <v>Figi</v>
       </c>
       <c r="K28" s="8" t="str">
-        <v>[More...]</v>
+        <v>ClientInternal</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -9670,22 +9733,22 @@
         <v>BBG007FAKECO</v>
       </c>
       <c r="F29" s="13" t="str">
-        <v>[More...]</v>
+        <v>Active</v>
       </c>
       <c r="G29" s="13" t="str">
-        <v>[More...]</v>
+        <v>LUID_A9RLV8U6</v>
       </c>
       <c r="H29" s="16" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="I29" s="16" t="str">
-        <v>[More...]</v>
+        <v>Spectre</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0</v>
       </c>
       <c r="J29" s="17" t="str">
-        <v>[More...]</v>
+        <v>BBG007FAKECO</v>
       </c>
       <c r="K29" s="17" t="str">
-        <v>[More...]</v>
+        <v>NewInst14</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -9695,23 +9758,23 @@
       <c r="C30" s="2"/>
       <c r="D30" s="9"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="G30" s="2" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="H30" s="2" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="I30" s="2" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="J30" s="2" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="K30" s="2" t="str">
-        <v>[More...]</v>
+      <c r="F30" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G30" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H30" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I30" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J30" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K30" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -9726,7 +9789,7 @@
       <c r="L31" s="50"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="18">
+  <dataValidations count="18">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Client supplied instrument Id" sqref="O17 O24" xr:uid="{00DDB5B9-AB50-4EB6-A9D1-57ADC0761B97}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument name" sqref="P17 P24" xr:uid="{12ED80DD-1447-4270-897B-A4131EB9C93A}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Type" sqref="Q17" xr:uid="{02C3AC28-C26B-4014-94BB-541E43E04CCA}"/>
@@ -9764,9 +9827,7 @@
   </sheetPr>
   <dimension ref="B1:N43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9812,7 +9873,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -9842,7 +9903,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -9858,7 +9919,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -9874,7 +9935,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -9952,7 +10013,7 @@
     <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -9970,7 +10031,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -9988,25 +10049,25 @@
       <c r="C15" s="2"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="K15" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>292</v>
       </c>
       <c r="L15" s="6" t="str">
         <f t="array" ref="L15:L17">_xll.flPropertiesAdd(E15:K17)</f>
@@ -10022,10 +10083,10 @@
         <v>219</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="H16" s="12" t="b">
         <v>0</v>
@@ -10035,10 +10096,10 @@
         <v>PlanType</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="L16" s="32" t="str">
         <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/PlanType' because it already exists.</v>
@@ -10053,22 +10114,22 @@
         <v>219</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="H17" s="43" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="J17" s="44" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="L17" s="32" t="str">
         <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/TakeOverWorldDate' because it already exists.</v>
@@ -10168,7 +10229,7 @@
     <row r="25" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
       <c r="C25" s="10" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -10186,7 +10247,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -10207,13 +10268,13 @@
         <v>221</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -10230,21 +10291,21 @@
       </c>
       <c r="E28" s="15" t="str">
         <f>'Add instrument'!G29</f>
-        <v>[More...]</v>
-      </c>
-      <c r="F28" s="46" t="s">
-        <v>340</v>
+        <v>LUID_A9RLV8U6</v>
+      </c>
+      <c r="F28" s="48">
+        <v>43101</v>
       </c>
       <c r="G28" s="43" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="H28" s="46" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="I28" s="42"/>
       <c r="J28" s="47" t="str">
         <f>_xll.flInstrumentPropertiesAdd(E27:H28)</f>
-        <v>#ERROR: A LusidInstrumentId must start with 'LUID_', or 'CCY_'.</v>
+        <v>OK</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -10333,7 +10394,7 @@
     <row r="34" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B34" s="2"/>
       <c r="C34" s="10" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -10351,7 +10412,7 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -10437,10 +10498,10 @@
         <v>PlanType</v>
       </c>
       <c r="K39" s="8" t="str">
-        <v/>
+        <v>Figi</v>
       </c>
       <c r="L39" s="8" t="str">
-        <v/>
+        <v>ClientInternal</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -10451,28 +10512,28 @@
       <c r="D40" s="9"/>
       <c r="E40" s="15" t="str">
         <f>E28</f>
-        <v>[More...]</v>
+        <v>LUID_A9RLV8U6</v>
       </c>
       <c r="F40" s="43" t="str">
-        <v/>
+        <v>Active</v>
       </c>
       <c r="G40" s="43" t="str">
-        <v/>
+        <v>LUID_A9RLV8U6</v>
       </c>
       <c r="H40" s="42" t="str">
-        <v/>
+        <v>Spectre</v>
       </c>
       <c r="I40" s="42" t="str">
-        <v/>
+        <v>2028/12/01T00:00:00.00</v>
       </c>
       <c r="J40" s="42" t="str">
-        <v/>
+        <v>Laser from satellite</v>
       </c>
       <c r="K40" s="42" t="str">
-        <v/>
+        <v>BBG007FAKECO</v>
       </c>
       <c r="L40" s="42" t="str">
-        <v/>
+        <v>NewInst14</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -10555,8 +10616,8 @@
   </sheetPr>
   <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10570,8 +10631,8 @@
     <col min="7" max="10" width="18.28515625" style="23" customWidth="1"/>
     <col min="11" max="11" width="22.7109375" style="23" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" style="23" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="23" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="23" customWidth="1"/>
     <col min="15" max="15" width="15.28515625" style="23" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.42578125" style="23" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="19.42578125" style="23" bestFit="1" customWidth="1"/>
@@ -10830,7 +10891,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -10961,7 +11022,7 @@
       <c r="T20"/>
       <c r="U20"/>
     </row>
-    <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -10987,13 +11048,15 @@
         <v>198</v>
       </c>
       <c r="L21" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="M21" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="N21" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="N21" s="2"/>
-      <c r="O21"/>
+      <c r="O21" s="2"/>
       <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
@@ -11002,7 +11065,7 @@
       <c r="U21" s="19"/>
       <c r="V21" s="19"/>
     </row>
-    <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
@@ -11022,16 +11085,16 @@
       <c r="J22" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K22" s="20" t="s">
-        <v>317</v>
+      <c r="K22" s="20">
+        <v>43570</v>
       </c>
       <c r="L22" s="20"/>
-      <c r="M22" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E22,F22,G22,H22,I22,J22,K22)</f>
-        <v>199.23</v>
-      </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="25"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E22,G22,H22,I22,J22,K22,L22,M22)</f>
+        <v>100</v>
+      </c>
+      <c r="O22" s="2"/>
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22"/>
@@ -11060,16 +11123,17 @@
       <c r="J23" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K23" s="20" t="s">
-        <v>323</v>
+      <c r="K23" s="20">
+        <f>K22+1</f>
+        <v>43571</v>
       </c>
       <c r="L23" s="20"/>
-      <c r="M23" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E23,F23,G23,H23,I23,J23,K23)</f>
+      <c r="M23" s="20"/>
+      <c r="N23" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E23,G23,H23,I23,J23,K23,L23,M23)</f>
         <v>199.25</v>
       </c>
-      <c r="N23" s="2"/>
-      <c r="O23" s="27"/>
+      <c r="O23" s="2"/>
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23"/>
@@ -11098,16 +11162,17 @@
       <c r="J24" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K24" s="20" t="s">
-        <v>324</v>
+      <c r="K24" s="20">
+        <f t="shared" ref="K24:K30" si="0">K23+1</f>
+        <v>43572</v>
       </c>
       <c r="L24" s="20"/>
-      <c r="M24" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E24,F24,G24,H24,I24,J24,K24)</f>
+      <c r="M24" s="20"/>
+      <c r="N24" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E24,G24,H24,I24,J24,K24,L24,M24)</f>
         <v>203.13</v>
       </c>
-      <c r="N24" s="2"/>
-      <c r="O24"/>
+      <c r="O24" s="2"/>
       <c r="P24"/>
       <c r="Q24"/>
       <c r="R24"/>
@@ -11136,16 +11201,17 @@
       <c r="J25" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K25" s="20" t="s">
-        <v>325</v>
+      <c r="K25" s="20">
+        <f t="shared" si="0"/>
+        <v>43573</v>
       </c>
       <c r="L25" s="20"/>
-      <c r="M25" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E25,F25,G25,H25,I25,J25,K25)</f>
+      <c r="M25" s="20"/>
+      <c r="N25" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E25,G25,H25,I25,J25,K25,L25,M25)</f>
         <v>203.86</v>
       </c>
-      <c r="N25" s="2"/>
-      <c r="O25"/>
+      <c r="O25" s="2"/>
       <c r="P25"/>
       <c r="Q25"/>
       <c r="R25"/>
@@ -11174,16 +11240,17 @@
       <c r="J26" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K26" s="20" t="s">
-        <v>326</v>
+      <c r="K26" s="20">
+        <f t="shared" si="0"/>
+        <v>43574</v>
       </c>
       <c r="L26" s="20"/>
-      <c r="M26" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E26,F26,G26,H26,I26,J26,K26)</f>
+      <c r="M26" s="20"/>
+      <c r="N26" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E26,G26,H26,I26,J26,K26,L26,M26)</f>
         <v>203.86</v>
       </c>
-      <c r="N26" s="2"/>
-      <c r="O26"/>
+      <c r="O26" s="2"/>
       <c r="P26"/>
       <c r="Q26"/>
       <c r="R26"/>
@@ -11209,16 +11276,17 @@
       <c r="J27" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K27" s="20" t="s">
-        <v>327</v>
+      <c r="K27" s="20">
+        <f t="shared" si="0"/>
+        <v>43575</v>
       </c>
       <c r="L27" s="20"/>
-      <c r="M27" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E27,F27,G27,H27,I27,J27,K27)</f>
+      <c r="M27" s="20"/>
+      <c r="N27" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E27,G27,H27,I27,J27,K27,L27,M27)</f>
         <v>203.86</v>
       </c>
-      <c r="N27" s="2"/>
-      <c r="O27"/>
+      <c r="O27" s="2"/>
       <c r="P27"/>
       <c r="Q27"/>
       <c r="R27"/>
@@ -11244,16 +11312,17 @@
       <c r="J28" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K28" s="20" t="s">
-        <v>328</v>
+      <c r="K28" s="20">
+        <f t="shared" si="0"/>
+        <v>43576</v>
       </c>
       <c r="L28" s="20"/>
-      <c r="M28" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E28,F28,G28,H28,I28,J28,K28)</f>
+      <c r="M28" s="20"/>
+      <c r="N28" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E28,G28,H28,I28,J28,K28,L28,M28)</f>
         <v>203.86</v>
       </c>
-      <c r="N28" s="2"/>
-      <c r="O28"/>
+      <c r="O28" s="2"/>
       <c r="P28"/>
       <c r="Q28"/>
       <c r="R28"/>
@@ -11279,16 +11348,17 @@
       <c r="J29" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K29" s="20" t="s">
-        <v>329</v>
+      <c r="K29" s="20">
+        <f t="shared" si="0"/>
+        <v>43577</v>
       </c>
       <c r="L29" s="20"/>
-      <c r="M29" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E29,F29,G29,H29,I29,J29,K29)</f>
+      <c r="M29" s="20"/>
+      <c r="N29" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E29,G29,H29,I29,J29,K29,L29,M29)</f>
         <v>204.53</v>
       </c>
-      <c r="N29" s="2"/>
-      <c r="O29"/>
+      <c r="O29" s="2"/>
       <c r="P29"/>
       <c r="Q29"/>
       <c r="R29"/>
@@ -11314,16 +11384,17 @@
       <c r="J30" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K30" s="20" t="s">
-        <v>330</v>
+      <c r="K30" s="20">
+        <f t="shared" si="0"/>
+        <v>43578</v>
       </c>
       <c r="L30" s="20"/>
-      <c r="M30" s="24">
-        <f>_xll.flQuoteGetForDate($F$15,E30,F30,G30,H30,I30,J30,K30)</f>
+      <c r="M30" s="20"/>
+      <c r="N30" s="52">
+        <f>_xll.flQuoteGetForDate($F$15,E30,G30,H30,I30,J30,K30,L30,M30)</f>
         <v>207.48</v>
       </c>
-      <c r="N30" s="2"/>
-      <c r="O30"/>
+      <c r="O30" s="2"/>
       <c r="P30"/>
       <c r="Q30"/>
       <c r="R30"/>
@@ -11341,9 +11412,9 @@
       <c r="J31" s="17"/>
       <c r="K31" s="20"/>
       <c r="L31" s="17"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="2"/>
-      <c r="O31"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="2"/>
       <c r="P31"/>
       <c r="Q31"/>
       <c r="R31"/>
@@ -11363,7 +11434,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32"/>
+      <c r="O32" s="2"/>
       <c r="P32"/>
       <c r="Q32"/>
       <c r="R32"/>
@@ -11412,8 +11483,8 @@
   </sheetPr>
   <dimension ref="B1:V34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11641,7 +11712,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -11784,13 +11855,13 @@
       <c r="J22" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K22" s="20" t="s">
-        <v>317</v>
+      <c r="K22" s="20">
+        <v>43570</v>
       </c>
       <c r="L22" s="20"/>
       <c r="M22" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E22,F22,G22,H22,I22,J22,K22)</f>
-        <v>199.23</v>
+        <f>_xll.flQuoteGetForDate($F$15,E22,G22,H22,I22,J22,K22,F22,L22)</f>
+        <v>100</v>
       </c>
       <c r="N22" s="2"/>
       <c r="T22" s="19"/>
@@ -11817,13 +11888,13 @@
       <c r="J23" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K23" s="20" t="s">
-        <v>317</v>
+      <c r="K23" s="20">
+        <v>43571</v>
       </c>
       <c r="L23" s="17"/>
       <c r="M23" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E23,F23,G23,H23,I23,J23,K23)</f>
-        <v>109.94</v>
+        <f>_xll.flQuoteGetForDate($F$15,E23,G23,H23,I23,J23,K23,F23,L23)</f>
+        <v>111.1</v>
       </c>
       <c r="N23" s="2"/>
       <c r="T23" s="19"/>
@@ -11850,13 +11921,13 @@
       <c r="J24" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K24" s="20" t="s">
-        <v>317</v>
+      <c r="K24" s="20">
+        <v>43572</v>
       </c>
       <c r="L24" s="17"/>
       <c r="M24" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E24,F24,G24,H24,I24,J24,K24)</f>
-        <v>78.63</v>
+        <f>_xll.flQuoteGetForDate($F$15,E24,G24,H24,I24,J24,K24,F24,L24)</f>
+        <v>78.36</v>
       </c>
       <c r="N24" s="2"/>
       <c r="T24" s="19"/>
@@ -11883,13 +11954,13 @@
       <c r="J25" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K25" s="20" t="s">
-        <v>317</v>
+      <c r="K25" s="20">
+        <v>43573</v>
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E25,F25,G25,H25,I25,J25,K25)</f>
-        <v>158.5</v>
+        <f>_xll.flQuoteGetForDate($F$15,E25,G25,H25,I25,J25,K25,F25,L25)</f>
+        <v>166.6</v>
       </c>
       <c r="N25" s="2"/>
       <c r="P25"/>
@@ -11917,13 +11988,13 @@
       <c r="J26" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K26" s="20" t="s">
-        <v>317</v>
+      <c r="K26" s="20">
+        <v>43574</v>
       </c>
       <c r="L26" s="17"/>
       <c r="M26" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E26,F26,G26,H26,I26,J26,K26)</f>
-        <v>655.9</v>
+        <f>_xll.flQuoteGetForDate($F$15,E26,G26,H26,I26,J26,K26,F26,L26)</f>
+        <v>666.5</v>
       </c>
       <c r="N26" s="2"/>
       <c r="P26"/>
@@ -11948,13 +12019,13 @@
       <c r="J27" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K27" s="20" t="s">
-        <v>317</v>
+      <c r="K27" s="20">
+        <v>43575</v>
       </c>
       <c r="L27" s="17"/>
       <c r="M27" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E27,F27,G27,H27,I27,J27,K27)</f>
-        <v>132.04</v>
+        <f>_xll.flQuoteGetForDate($F$15,E27,G27,H27,I27,J27,K27,F27,L27)</f>
+        <v>132.44999999999999</v>
       </c>
       <c r="N27" s="2"/>
       <c r="P27"/>
@@ -11979,13 +12050,13 @@
       <c r="J28" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K28" s="20" t="s">
-        <v>317</v>
+      <c r="K28" s="20">
+        <v>43576</v>
       </c>
       <c r="L28" s="17"/>
       <c r="M28" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E28,F28,G28,H28,I28,J28,K28)</f>
-        <v>121.05</v>
+        <f>_xll.flQuoteGetForDate($F$15,E28,G28,H28,I28,J28,K28,F28,L28)</f>
+        <v>123.37</v>
       </c>
       <c r="N28" s="2"/>
       <c r="P28"/>
@@ -12010,13 +12081,13 @@
       <c r="J29" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K29" s="20" t="s">
-        <v>317</v>
+      <c r="K29" s="20">
+        <v>43577</v>
       </c>
       <c r="L29" s="17"/>
       <c r="M29" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E29,F29,G29,H29,I29,J29,K29)</f>
-        <v>6831</v>
+        <f>_xll.flQuoteGetForDate($F$15,E29,G29,H29,I29,J29,K29,F29,L29)</f>
+        <v>6963</v>
       </c>
       <c r="N29" s="2"/>
       <c r="P29"/>
@@ -12041,13 +12112,13 @@
       <c r="J30" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K30" s="20" t="s">
-        <v>317</v>
+      <c r="K30" s="20">
+        <v>43578</v>
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E30,F30,G30,H30,I30,J30,K30)</f>
-        <v>569.9</v>
+        <f>_xll.flQuoteGetForDate($F$15,E30,G30,H30,I30,J30,K30,F30,L30)</f>
+        <v>582.5</v>
       </c>
       <c r="N30" s="2"/>
       <c r="P30"/>
@@ -12072,13 +12143,13 @@
       <c r="J31" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K31" s="20" t="s">
-        <v>317</v>
+      <c r="K31" s="20">
+        <v>43579</v>
       </c>
       <c r="L31" s="17"/>
       <c r="M31" s="17">
-        <f>_xll.flQuoteGetForDate($F$15,E31,F31,G31,H31,I31,J31,K31)</f>
-        <v>11825</v>
+        <f>_xll.flQuoteGetForDate($F$15,E31,G31,H31,I31,J31,K31,F31,L31)</f>
+        <v>11550</v>
       </c>
       <c r="N31" s="2"/>
       <c r="P31"/>
@@ -12118,6 +12189,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005F4F0FA1AC8B142BA5BFAEE01329AF1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="51d44e6750016a81140edd9302933050">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7f1325bc-d786-4e92-924e-74ffe34b2b40" xmlns:ns3="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbbf5b69800df541767d824f3fbf5177" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -12343,15 +12423,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12363,6 +12434,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45EDF347-3168-4BEB-9A6E-9322773C07F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12382,28 +12461,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F07F7B26-A8FB-44CC-BC1A-494CF9683469}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DEV-4675 made some cosmetic changes for MR
</commit_message>
<xml_diff>
--- a/LUSID Excel - Setting up your market data.xlsx
+++ b/LUSID Excel - Setting up your market data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusSekhon\Dev\sample-excel\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EB7FBF-3ACC-49D7-8111-6ACF3B5E5CF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47717318-48EF-4C7A-9258-F8C5613B5CB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" firstSheet="1" activeTab="5" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
+    <workbookView xWindow="-28920" yWindow="255" windowWidth="29040" windowHeight="15840" tabRatio="798" activeTab="6" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Datetime format" sheetId="21" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <definedName name="fbnHoldings_Template_ref" localSheetId="8">'List prices 2'!#REF!</definedName>
     <definedName name="fbnHoldings_Template_ref" localSheetId="9">'Update prices'!$E$20:$L$20</definedName>
     <definedName name="fbnInstrumentProperties_Template_ref" localSheetId="5">'Add instrument'!$G$42:$H$42</definedName>
-    <definedName name="fbnInstrumentProperties_Template_ref" localSheetId="6">'Add property definition'!$G$22:$H$22</definedName>
+    <definedName name="fbnInstrumentProperties_Template_ref" localSheetId="6">'Add property definition'!$G$23:$H$23</definedName>
     <definedName name="fbnInstrumentProperties_Template_ref" localSheetId="4">'Edit instrument'!$E$44:$F$44</definedName>
     <definedName name="fbnInstrumentProperties_Template_ref" localSheetId="3">'Get instrument definition'!#REF!</definedName>
     <definedName name="fbnInstrumentProperties_Template_ref" localSheetId="1">'List identifiers'!#REF!</definedName>
@@ -85,7 +85,7 @@
     <definedName name="fbnInstruments_Template_ref" localSheetId="1">'List identifiers'!#REF!</definedName>
     <definedName name="fbnInstruments_Template_ref" localSheetId="2">'List instruments'!#REF!</definedName>
     <definedName name="fbnPropertiesAdd_Template_ref" localSheetId="5">'Add instrument'!$G$38:$M$38</definedName>
-    <definedName name="fbnPropertiesAdd_Template_ref" localSheetId="6">'Add property definition'!$G$18:$M$18</definedName>
+    <definedName name="fbnPropertiesAdd_Template_ref" localSheetId="6">'Add property definition'!$G$19:$M$19</definedName>
     <definedName name="fbnPropertiesAdd_Template_ref" localSheetId="4">'Edit instrument'!#REF!</definedName>
     <definedName name="fbnPropertiesAdd_Template_ref" localSheetId="3">'Get instrument definition'!$N$32:$U$32</definedName>
     <definedName name="fbnPropertiesAdd_Template_ref" localSheetId="1">'List identifiers'!$N$28:$U$28</definedName>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="337">
   <si>
     <t>Base Currency</t>
   </si>
@@ -1116,9 +1116,6 @@
     <t>some-format</t>
   </si>
   <si>
-    <t>In this case we are adding an instrument definition format. Don’t forget you can use the flInstrumentsAdd_Template to see a list of the required fields</t>
-  </si>
-  <si>
     <t>Effective From</t>
   </si>
   <si>
@@ -1165,6 +1162,15 @@
   </si>
   <si>
     <t>Identifier</t>
+  </si>
+  <si>
+    <t>Properties...</t>
+  </si>
+  <si>
+    <t>In this case we are adding instrument properties. Don’t forget you can use the template to see a list of the required fields. Click on the returned cells to see tooltips</t>
+  </si>
+  <si>
+    <t>In this case we are adding an instrument definition format. Don’t forget you can use the flInstrumentsAdd_Template to see a list of the required fields. Click on the returned cells to see tooltips</t>
   </si>
 </sst>
 </file>
@@ -1425,9 +1431,6 @@
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1470,6 +1473,9 @@
     <xf numFmtId="4" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1500,359 +1506,344 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>a21dcc50-2da3-4263-80f8-751d4144b1f6</stp>
-        <tr r="M23" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>44531640-76af-4bae-a970-b5e1d2a0fa4f</stp>
-        <tr r="G29" s="14"/>
-        <tr r="K30" s="14"/>
-        <tr r="F28" s="14"/>
-        <tr r="I30" s="14"/>
-        <tr r="F29" s="14"/>
-        <tr r="H29" s="14"/>
-        <tr r="K28" s="14"/>
-        <tr r="H30" s="14"/>
-        <tr r="G28" s="14"/>
-        <tr r="I29" s="14"/>
-        <tr r="K29" s="14"/>
-        <tr r="J30" s="14"/>
-        <tr r="H28" s="14"/>
-        <tr r="J28" s="14"/>
-        <tr r="I28" s="14"/>
-        <tr r="J29" s="14"/>
-        <tr r="F30" s="14"/>
-        <tr r="G30" s="14"/>
+        <stp>c50cb65d-7357-4bba-925b-0e6f6a96cb6e</stp>
+        <tr r="N25" s="16"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>96cf756f-cab3-499f-a8bb-8b67d68e911b</stp>
-        <tr r="M29" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>37951179-1d80-4f86-93b4-1f5f4cb35fe4</stp>
-        <tr r="G34" s="13"/>
-        <tr r="H35" s="13"/>
-        <tr r="I34" s="13"/>
-        <tr r="J34" s="13"/>
-        <tr r="F35" s="13"/>
-        <tr r="I36" s="13"/>
-        <tr r="H36" s="13"/>
-        <tr r="G36" s="13"/>
-        <tr r="F34" s="13"/>
-        <tr r="K34" s="13"/>
-        <tr r="F36" s="13"/>
-        <tr r="K35" s="13"/>
-        <tr r="J35" s="13"/>
-        <tr r="H34" s="13"/>
-        <tr r="J36" s="13"/>
-        <tr r="G35" s="13"/>
-        <tr r="I35" s="13"/>
-        <tr r="K36" s="13"/>
+        <stp>b435a4aa-6a55-4e9c-b311-b75536b39cfc</stp>
+        <tr r="M31" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>e6218218-b205-4d18-b844-e944cbb63158</stp>
+        <stp>ca279f9c-3e0c-4fb7-b7c5-1e093a6d1bcb</stp>
         <tr r="M24" s="17"/>
       </tp>
     </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>4b12e51d-d5cb-4b0e-92f2-5571df7d6e69</stp>
+        <stp>60b5e063-bb7a-4e71-b272-dc94ce5daa98</stp>
         <tr r="M22" s="17"/>
         <tr r="N22" s="16"/>
       </tp>
     </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>d7709217-a847-4050-bf37-dfa215753290</stp>
-        <tr r="I27" s="10"/>
-        <tr r="H21" s="10"/>
-        <tr r="K30" s="10"/>
-        <tr r="H29" s="10"/>
-        <tr r="G24" s="10"/>
-        <tr r="J29" s="10"/>
-        <tr r="I29" s="10"/>
-        <tr r="G30" s="10"/>
-        <tr r="G22" s="10"/>
-        <tr r="I21" s="10"/>
-        <tr r="K21" s="10"/>
-        <tr r="F29" s="10"/>
-        <tr r="I24" s="10"/>
-        <tr r="I26" s="10"/>
-        <tr r="F24" s="10"/>
-        <tr r="F26" s="10"/>
-        <tr r="J22" s="10"/>
-        <tr r="K23" s="10"/>
-        <tr r="H26" s="10"/>
-        <tr r="G31" s="10"/>
-        <tr r="K25" s="10"/>
-        <tr r="F30" s="10"/>
-        <tr r="I23" s="10"/>
-        <tr r="H23" s="10"/>
-        <tr r="K29" s="10"/>
-        <tr r="K24" s="10"/>
-        <tr r="K31" s="10"/>
-        <tr r="J25" s="10"/>
-        <tr r="K28" s="10"/>
-        <tr r="I28" s="10"/>
-        <tr r="H25" s="10"/>
-        <tr r="I25" s="10"/>
-        <tr r="G28" s="10"/>
-        <tr r="J27" s="10"/>
-        <tr r="K26" s="10"/>
-        <tr r="F28" s="10"/>
-        <tr r="H28" s="10"/>
-        <tr r="H24" s="10"/>
-        <tr r="G27" s="10"/>
-        <tr r="H27" s="10"/>
-        <tr r="I22" s="10"/>
-        <tr r="G23" s="10"/>
-        <tr r="H31" s="10"/>
-        <tr r="H30" s="10"/>
-        <tr r="F22" s="10"/>
-        <tr r="J26" s="10"/>
-        <tr r="G26" s="10"/>
-        <tr r="F23" s="10"/>
-        <tr r="J31" s="10"/>
-        <tr r="F21" s="10"/>
-        <tr r="K22" s="10"/>
-        <tr r="J23" s="10"/>
-        <tr r="F27" s="10"/>
-        <tr r="G25" s="10"/>
-        <tr r="J21" s="10"/>
-        <tr r="G21" s="10"/>
-        <tr r="I30" s="10"/>
-        <tr r="F25" s="10"/>
-        <tr r="J28" s="10"/>
-        <tr r="K27" s="10"/>
-        <tr r="G29" s="10"/>
-        <tr r="I31" s="10"/>
-        <tr r="H22" s="10"/>
-        <tr r="J24" s="10"/>
-        <tr r="J30" s="10"/>
-        <tr r="F31" s="10"/>
+        <stp>8522b8df-70ef-42e9-b230-53d7812b918d</stp>
+        <tr r="M28" s="17"/>
       </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>244bb2e4-23a6-46ae-b209-9d3c662f363f</stp>
+        <stp>c5240d04-6a2a-412a-9ce9-45651707aa35</stp>
+        <tr r="M27" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>254a7417-71c0-4d0b-97da-4ef09baf164c</stp>
+        <tr r="M26" s="17"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>8fc2746e-0bc6-4fb4-88f5-28b9c04f4935</stp>
         <tr r="N23" s="16"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>7d2717eb-c97f-4176-b7cf-3c5436d9c596</stp>
-        <tr r="N30" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>16c0d930-6cf2-433a-8ed1-a422f5be84e8</stp>
-        <tr r="N24" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>62cf7019-35b3-4a4a-ba99-a0a67d2790ee</stp>
-        <tr r="M30" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>5eb375fe-3a7b-4421-a118-eebbe1eecd0f</stp>
-        <tr r="M28" s="17"/>
+        <stp>1b851d24-d423-40d8-a07d-cb22e791d9c2</stp>
+        <tr r="F29" s="14"/>
+        <tr r="G28" s="14"/>
+        <tr r="J30" s="14"/>
+        <tr r="K30" s="14"/>
+        <tr r="F28" s="14"/>
+        <tr r="I28" s="14"/>
+        <tr r="F30" s="14"/>
+        <tr r="G30" s="14"/>
+        <tr r="I30" s="14"/>
+        <tr r="I29" s="14"/>
+        <tr r="K28" s="14"/>
+        <tr r="K29" s="14"/>
+        <tr r="H28" s="14"/>
+        <tr r="H30" s="14"/>
+        <tr r="H29" s="14"/>
+        <tr r="J28" s="14"/>
+        <tr r="J29" s="14"/>
+        <tr r="G29" s="14"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>420da05c-b3a9-4db9-868f-8795024356e6</stp>
+        <stp>fabdc791-bebd-4068-a5f3-7587f67fff9d</stp>
+        <tr r="N30" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>f8a64455-60f3-4705-ab8d-60f78647c960</stp>
+        <tr r="N28" s="16"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>e0573e3b-e627-4647-ac21-19e443c88713</stp>
+        <tr r="N24" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>859dfc47-66cd-4db0-addb-10021f8ee460</stp>
+        <tr r="M29" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>47da3280-4fb8-4c80-bce1-505230dbd39a</stp>
+        <tr r="N29" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>39ad07fe-cb1c-414a-9b70-e94230d34f0c</stp>
         <tr r="M25" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>82a4b30f-137e-4aca-a0bb-2f56cffc6a77</stp>
-        <tr r="M27" s="17"/>
+        <stp>4cc8c981-9216-4d17-a471-1afb36919abc</stp>
+        <tr r="M30" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>93b03581-da2f-4af5-9a54-e7acf3fb730f</stp>
+        <tr r="N27" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>b4ab096c-c194-4d70-9688-cf60a5d03e48</stp>
+        <tr r="L42" s="20"/>
+        <tr r="F43" s="20"/>
+        <tr r="H43" s="20"/>
+        <tr r="F42" s="20"/>
+        <tr r="K43" s="20"/>
+        <tr r="G42" s="20"/>
+        <tr r="L43" s="20"/>
+        <tr r="J42" s="20"/>
+        <tr r="K42" s="20"/>
+        <tr r="I42" s="20"/>
+        <tr r="I43" s="20"/>
+        <tr r="J43" s="20"/>
+        <tr r="H42" s="20"/>
+        <tr r="G43" s="20"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>e9cde9fb-7f17-4338-82b5-1c0c22738bb5</stp>
+        <tr r="F26" s="12"/>
+        <tr r="E28" s="12"/>
+        <tr r="G33" s="12"/>
+        <tr r="F25" s="12"/>
+        <tr r="F23" s="12"/>
+        <tr r="E30" s="12"/>
+        <tr r="G28" s="12"/>
+        <tr r="F29" s="12"/>
+        <tr r="E27" s="12"/>
+        <tr r="F28" s="12"/>
+        <tr r="F24" s="12"/>
+        <tr r="G23" s="12"/>
+        <tr r="G31" s="12"/>
+        <tr r="G30" s="12"/>
+        <tr r="G29" s="12"/>
+        <tr r="E29" s="12"/>
+        <tr r="E33" s="12"/>
+        <tr r="F31" s="12"/>
+        <tr r="G24" s="12"/>
+        <tr r="E24" s="12"/>
+        <tr r="G27" s="12"/>
+        <tr r="F27" s="12"/>
+        <tr r="F33" s="12"/>
+        <tr r="E26" s="12"/>
+        <tr r="E32" s="12"/>
+        <tr r="F30" s="12"/>
+        <tr r="G32" s="12"/>
+        <tr r="G26" s="12"/>
+        <tr r="E25" s="12"/>
+        <tr r="E31" s="12"/>
+        <tr r="E23" s="12"/>
+        <tr r="G25" s="12"/>
+        <tr r="F32" s="12"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>b3cf1375-d7be-434a-8b0a-1604e65f3d69</stp>
-        <tr r="M26" s="17"/>
+        <stp>9e485a87-4f72-4786-8c89-1fccc11b466b</stp>
+        <tr r="N26" s="16"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>ae3e063a-c168-4ff8-8088-fb37ce6d2fee</stp>
-        <tr r="N29" s="16"/>
+        <stp>393ee071-10f6-429b-a08e-084623a825c0</stp>
+        <tr r="H36" s="13"/>
+        <tr r="J35" s="13"/>
+        <tr r="J34" s="13"/>
+        <tr r="G36" s="13"/>
+        <tr r="F34" s="13"/>
+        <tr r="G35" s="13"/>
+        <tr r="K35" s="13"/>
+        <tr r="H34" s="13"/>
+        <tr r="I35" s="13"/>
+        <tr r="F35" s="13"/>
+        <tr r="H35" s="13"/>
+        <tr r="G34" s="13"/>
+        <tr r="I34" s="13"/>
+        <tr r="K36" s="13"/>
+        <tr r="K34" s="13"/>
+        <tr r="I36" s="13"/>
+        <tr r="F36" s="13"/>
+        <tr r="J36" s="13"/>
       </tp>
     </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
+    <main first="rtdsrv.779f36d3706147749a58e1383e92c483">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>c0363e30-9e1e-4d38-9b6c-6b4eeaf3b161</stp>
-        <tr r="H40" s="20"/>
-        <tr r="F39" s="20"/>
-        <tr r="L39" s="20"/>
-        <tr r="L40" s="20"/>
-        <tr r="K39" s="20"/>
-        <tr r="I40" s="20"/>
-        <tr r="H39" s="20"/>
-        <tr r="G40" s="20"/>
-        <tr r="F40" s="20"/>
-        <tr r="K40" s="20"/>
-        <tr r="G39" s="20"/>
-        <tr r="J39" s="20"/>
-        <tr r="I39" s="20"/>
-        <tr r="J40" s="20"/>
+        <stp>7300f696-9d56-4190-920c-6f3605c31494</stp>
+        <tr r="I31" s="10"/>
+        <tr r="J28" s="10"/>
+        <tr r="I26" s="10"/>
+        <tr r="H29" s="10"/>
+        <tr r="I29" s="10"/>
+        <tr r="I27" s="10"/>
+        <tr r="J31" s="10"/>
+        <tr r="F30" s="10"/>
+        <tr r="G27" s="10"/>
+        <tr r="F25" s="10"/>
+        <tr r="G26" s="10"/>
+        <tr r="H26" s="10"/>
+        <tr r="I30" s="10"/>
+        <tr r="G30" s="10"/>
+        <tr r="H28" s="10"/>
+        <tr r="I25" s="10"/>
+        <tr r="H23" s="10"/>
+        <tr r="H21" s="10"/>
+        <tr r="G23" s="10"/>
+        <tr r="F29" s="10"/>
+        <tr r="I28" s="10"/>
+        <tr r="J26" s="10"/>
+        <tr r="F24" s="10"/>
+        <tr r="J21" s="10"/>
+        <tr r="G29" s="10"/>
+        <tr r="F31" s="10"/>
+        <tr r="H27" s="10"/>
+        <tr r="F27" s="10"/>
+        <tr r="G25" s="10"/>
+        <tr r="H22" s="10"/>
+        <tr r="G31" s="10"/>
+        <tr r="F26" s="10"/>
+        <tr r="J27" s="10"/>
+        <tr r="J25" s="10"/>
+        <tr r="H25" s="10"/>
+        <tr r="I23" s="10"/>
+        <tr r="H31" s="10"/>
+        <tr r="F28" s="10"/>
+        <tr r="H24" s="10"/>
+        <tr r="I24" s="10"/>
+        <tr r="G24" s="10"/>
+        <tr r="J23" s="10"/>
+        <tr r="F22" s="10"/>
+        <tr r="J29" s="10"/>
+        <tr r="J24" s="10"/>
+        <tr r="J22" s="10"/>
+        <tr r="F23" s="10"/>
+        <tr r="I22" s="10"/>
+        <tr r="G22" s="10"/>
+        <tr r="H30" s="10"/>
+        <tr r="G28" s="10"/>
+        <tr r="I21" s="10"/>
+        <tr r="G21" s="10"/>
+        <tr r="J30" s="10"/>
+        <tr r="F21" s="10"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>b0e72c9d-a4bd-4e04-a47d-d3881bf11772</stp>
-        <tr r="N25" s="16"/>
+        <stp>9ab13324-b31f-4966-ac8e-b12b7101de1b</stp>
+        <tr r="M23" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>8f35840b-2985-493e-85ff-251fa7001733</stp>
+        <stp>dd32a6f0-62af-473d-8919-4bf2c3de2829</stp>
+        <tr r="F27" s="11"/>
+        <tr r="F21" s="11"/>
+        <tr r="G19" s="11"/>
+        <tr r="G24" s="11"/>
+        <tr r="F19" s="11"/>
+        <tr r="F25" s="11"/>
+        <tr r="G22" s="11"/>
+        <tr r="E23" s="11"/>
+        <tr r="F26" s="11"/>
+        <tr r="E18" s="11"/>
+        <tr r="E28" s="11"/>
+        <tr r="F22" s="11"/>
+        <tr r="G27" s="11"/>
+        <tr r="E22" s="11"/>
+        <tr r="G20" s="11"/>
+        <tr r="G17" s="11"/>
+        <tr r="E29" s="11"/>
         <tr r="E26" s="11"/>
-        <tr r="G20" s="11"/>
+        <tr r="F18" s="11"/>
+        <tr r="E25" s="11"/>
         <tr r="G21" s="11"/>
-        <tr r="F25" s="11"/>
-        <tr r="F27" s="11"/>
+        <tr r="E20" s="11"/>
+        <tr r="E21" s="11"/>
+        <tr r="G18" s="11"/>
+        <tr r="F24" s="11"/>
+        <tr r="G23" s="11"/>
+        <tr r="F23" s="11"/>
+        <tr r="G28" s="11"/>
+        <tr r="G25" s="11"/>
+        <tr r="E19" s="11"/>
+        <tr r="G29" s="11"/>
+        <tr r="F28" s="11"/>
+        <tr r="E24" s="11"/>
+        <tr r="F20" s="11"/>
+        <tr r="F17" s="11"/>
         <tr r="E17" s="11"/>
-        <tr r="E28" s="11"/>
-        <tr r="G27" s="11"/>
-        <tr r="G18" s="11"/>
-        <tr r="G22" s="11"/>
-        <tr r="G17" s="11"/>
-        <tr r="F24" s="11"/>
-        <tr r="G19" s="11"/>
-        <tr r="F18" s="11"/>
-        <tr r="G23" s="11"/>
         <tr r="G26" s="11"/>
-        <tr r="F23" s="11"/>
-        <tr r="F28" s="11"/>
-        <tr r="G24" s="11"/>
-        <tr r="E23" s="11"/>
-        <tr r="E20" s="11"/>
-        <tr r="F17" s="11"/>
-        <tr r="F26" s="11"/>
-        <tr r="F22" s="11"/>
-        <tr r="E29" s="11"/>
-        <tr r="E21" s="11"/>
-        <tr r="G28" s="11"/>
-        <tr r="F21" s="11"/>
-        <tr r="F19" s="11"/>
-        <tr r="E25" s="11"/>
-        <tr r="E18" s="11"/>
-        <tr r="G25" s="11"/>
-        <tr r="E24" s="11"/>
         <tr r="E27" s="11"/>
-        <tr r="E19" s="11"/>
         <tr r="F29" s="11"/>
-        <tr r="E22" s="11"/>
-        <tr r="G29" s="11"/>
-        <tr r="F20" s="11"/>
-      </tp>
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>19b75e0e-ea82-4fca-9c13-9582f8e1c1e4</stp>
-        <tr r="N27" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>7dd92585-a569-455b-802e-f07393b52735</stp>
-        <tr r="F27" s="12"/>
-        <tr r="E25" s="12"/>
-        <tr r="G25" s="12"/>
-        <tr r="F23" s="12"/>
-        <tr r="G32" s="12"/>
-        <tr r="E23" s="12"/>
-        <tr r="G33" s="12"/>
-        <tr r="E33" s="12"/>
-        <tr r="G24" s="12"/>
-        <tr r="F26" s="12"/>
-        <tr r="F25" s="12"/>
-        <tr r="E24" s="12"/>
-        <tr r="F32" s="12"/>
-        <tr r="F29" s="12"/>
-        <tr r="E28" s="12"/>
-        <tr r="E27" s="12"/>
-        <tr r="G31" s="12"/>
-        <tr r="F31" s="12"/>
-        <tr r="G29" s="12"/>
-        <tr r="F33" s="12"/>
-        <tr r="G27" s="12"/>
-        <tr r="F28" s="12"/>
-        <tr r="E26" s="12"/>
-        <tr r="G26" s="12"/>
-        <tr r="G30" s="12"/>
-        <tr r="E32" s="12"/>
-        <tr r="E30" s="12"/>
-        <tr r="F24" s="12"/>
-        <tr r="E29" s="12"/>
-        <tr r="F30" s="12"/>
-        <tr r="E31" s="12"/>
-        <tr r="G28" s="12"/>
-        <tr r="G23" s="12"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>0e94f185-2ca1-47c8-a339-5c93fdd7e222</stp>
-        <tr r="M31" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>773b0084-37d8-480a-a7e3-5023681d3d42</stp>
-        <tr r="N26" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>c22cd5cb-707d-4297-925f-a9ac2a54a6e2</stp>
-        <tr r="N28" s="16"/>
       </tp>
     </main>
   </volType>
@@ -2921,7 +2912,7 @@
   <dimension ref="B1:T31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,12 +3100,12 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -3145,12 +3136,12 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -3190,7 +3181,7 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I17" s="25" t="s">
         <v>308</v>
@@ -3235,7 +3226,7 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I19" s="25" t="str">
         <f>TEXT(F23,"yyyy-mm-dd")&amp;"T"&amp;TEXT(F23," hh:mm:ss.00Z")</f>
@@ -3278,12 +3269,12 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I21" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="I21" s="25" t="s">
-        <v>328</v>
-      </c>
-      <c r="J21" s="50"/>
+      <c r="J21" s="49"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -3321,7 +3312,7 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I23" s="25" t="str">
         <f>TEXT(F23,"yyyy-mm-dd")&amp;"NSingaporeClose"</f>
@@ -3392,7 +3383,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F27" s="30">
         <f>F23+1/24</f>
@@ -3429,7 +3420,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F29" s="30">
         <f>F27-1/1440</f>
@@ -4061,7 +4052,7 @@
         <v>213</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>204</v>
@@ -4084,9 +4075,9 @@
       <c r="M23" s="20">
         <v>43570</v>
       </c>
-      <c r="N23" s="47"/>
+      <c r="N23" s="46"/>
       <c r="O23" s="32"/>
-      <c r="P23" s="51" t="str">
+      <c r="P23" s="50" t="str">
         <f>_xll.flQuotesAdd(F15,E22:O23)</f>
         <v>Added 1 quote(s) as at time 2019-09-03 16:02:48Z</v>
       </c>
@@ -4120,7 +4111,7 @@
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
-      <c r="P24" s="51"/>
+      <c r="P24" s="50"/>
       <c r="Q24" s="2"/>
       <c r="R24"/>
       <c r="S24"/>
@@ -4151,7 +4142,7 @@
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
-      <c r="P25" s="51"/>
+      <c r="P25" s="50"/>
       <c r="Q25" s="2"/>
       <c r="R25"/>
       <c r="S25"/>
@@ -4182,7 +4173,7 @@
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
-      <c r="P26" s="51"/>
+      <c r="P26" s="50"/>
       <c r="Q26" s="2"/>
       <c r="R26"/>
       <c r="S26"/>
@@ -4213,7 +4204,7 @@
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
-      <c r="P27" s="51"/>
+      <c r="P27" s="50"/>
       <c r="Q27" s="2"/>
       <c r="R27"/>
       <c r="S27"/>
@@ -4244,7 +4235,7 @@
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
-      <c r="P28" s="51"/>
+      <c r="P28" s="50"/>
       <c r="Q28" s="2"/>
       <c r="R28"/>
       <c r="S28"/>
@@ -4275,7 +4266,7 @@
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
-      <c r="P29" s="51"/>
+      <c r="P29" s="50"/>
       <c r="Q29" s="2"/>
       <c r="R29"/>
       <c r="S29"/>
@@ -4401,10 +4392,10 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="41"/>
-      <c r="Q34" s="41"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
       <c r="R34"/>
       <c r="S34"/>
       <c r="T34"/>
@@ -5342,7 +5333,7 @@
       </c>
       <c r="N24" s="32"/>
       <c r="O24" s="32"/>
-      <c r="P24" s="51" t="str">
+      <c r="P24" s="50" t="str">
         <f>_xll.flQuotesAdd(F15,E23:O27)</f>
         <v>Added 4 quote(s) as at time 2019-09-03 16:02:48Z</v>
       </c>
@@ -5390,7 +5381,7 @@
       </c>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
-      <c r="P25" s="51"/>
+      <c r="P25" s="50"/>
       <c r="Q25" s="2"/>
       <c r="R25"/>
       <c r="S25"/>
@@ -5435,7 +5426,7 @@
       </c>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
-      <c r="P26" s="51"/>
+      <c r="P26" s="50"/>
       <c r="Q26" s="2"/>
       <c r="R26"/>
       <c r="S26"/>
@@ -5480,7 +5471,7 @@
       </c>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
-      <c r="P27" s="51"/>
+      <c r="P27" s="50"/>
       <c r="Q27" s="2"/>
       <c r="R27"/>
       <c r="S27"/>
@@ -6656,7 +6647,7 @@
   <dimension ref="B1:R30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6859,7 +6850,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -6872,16 +6863,12 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>204</v>
-      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -6951,14 +6938,14 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="37" t="str">
-        <v>Figi</v>
+      <c r="E19" s="36" t="str">
+        <v>ShareClassFigi</v>
       </c>
       <c r="F19" s="18" t="str">
-        <v>Instrument/default/Figi</v>
+        <v>Instrument/default/ShareClassFigi</v>
       </c>
       <c r="G19" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -6973,11 +6960,11 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="37" t="str">
-        <v>Cusip</v>
+      <c r="E20" s="36" t="str">
+        <v>CompositeFigi</v>
       </c>
       <c r="F20" s="18" t="str">
-        <v>Instrument/default/Cusip</v>
+        <v>Instrument/default/CompositeFigi</v>
       </c>
       <c r="G20" s="18" t="b">
         <v>0</v>
@@ -6995,14 +6982,14 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="37" t="str">
-        <v>RIC</v>
+      <c r="E21" s="36" t="str">
+        <v>QuotePermId</v>
       </c>
       <c r="F21" s="18" t="str">
-        <v>Instrument/default/RIC</v>
+        <v>Instrument/default/QuotePermId</v>
       </c>
       <c r="G21" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -7017,14 +7004,14 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="37" t="str">
-        <v>Ticker</v>
+      <c r="E22" s="36" t="str">
+        <v>LusidInstrumentId</v>
       </c>
       <c r="F22" s="18" t="str">
-        <v>Instrument/default/Ticker</v>
+        <v>Instrument/default/LusidInstrumentId</v>
       </c>
       <c r="G22" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -7039,14 +7026,14 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="37" t="str">
-        <v>LusidInstrumentId</v>
+      <c r="E23" s="36" t="str">
+        <v>RIC</v>
       </c>
       <c r="F23" s="18" t="str">
-        <v>Instrument/default/LusidInstrumentId</v>
+        <v>Instrument/default/RIC</v>
       </c>
       <c r="G23" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -7061,14 +7048,14 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="37" t="str">
-        <v>ClientInternal</v>
+      <c r="E24" s="36" t="str">
+        <v>Ticker</v>
       </c>
       <c r="F24" s="18" t="str">
-        <v>Instrument/default/ClientInternal</v>
+        <v>Instrument/default/Ticker</v>
       </c>
       <c r="G24" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -7082,11 +7069,11 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="37" t="str">
-        <v>ShareClassFigi</v>
+      <c r="E25" s="36" t="str">
+        <v>Cusip</v>
       </c>
       <c r="F25" s="18" t="str">
-        <v>Instrument/default/ShareClassFigi</v>
+        <v>Instrument/default/Cusip</v>
       </c>
       <c r="G25" s="18" t="b">
         <v>0</v>
@@ -7101,11 +7088,11 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="37" t="str">
-        <v>QuotePermId</v>
+      <c r="E26" s="36" t="str">
+        <v>Figi</v>
       </c>
       <c r="F26" s="18" t="str">
-        <v>Instrument/default/QuotePermId</v>
+        <v>Instrument/default/Figi</v>
       </c>
       <c r="G26" s="18" t="b">
         <v>1</v>
@@ -7120,14 +7107,14 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="37" t="str">
-        <v>CompositeFigi</v>
+      <c r="E27" s="36" t="str">
+        <v>ClientInternal</v>
       </c>
       <c r="F27" s="18" t="str">
-        <v>Instrument/default/CompositeFigi</v>
+        <v>Instrument/default/ClientInternal</v>
       </c>
       <c r="G27" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -7139,7 +7126,7 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="37" t="str">
+      <c r="E28" s="36" t="str">
         <v>Wertpapier</v>
       </c>
       <c r="F28" s="18" t="str">
@@ -7158,7 +7145,7 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="37" t="str">
+      <c r="E29" s="36" t="str">
         <v>Isin</v>
       </c>
       <c r="F29" s="18" t="str">
@@ -7481,12 +7468,12 @@
       <c r="D21" s="9"/>
       <c r="E21" s="25">
         <f ca="1">NOW()</f>
-        <v>43712.699978009259</v>
+        <v>43718.477425925928</v>
       </c>
       <c r="F21" s="25">
         <v>43697</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G21" s="47">
         <v>5</v>
       </c>
       <c r="H21" s="2"/>
@@ -7556,7 +7543,7 @@
       <c r="D25" s="2">
         <v>2</v>
       </c>
-      <c r="E25" s="37" t="str">
+      <c r="E25" s="36" t="str">
         <f ca="1"/>
         <v>Active</v>
       </c>
@@ -7579,7 +7566,7 @@
       <c r="D26" s="2">
         <v>3</v>
       </c>
-      <c r="E26" s="37" t="str">
+      <c r="E26" s="36" t="str">
         <f ca="1"/>
         <v>Active</v>
       </c>
@@ -7602,7 +7589,7 @@
       <c r="D27" s="2">
         <v>4</v>
       </c>
-      <c r="E27" s="37" t="str">
+      <c r="E27" s="36" t="str">
         <f ca="1"/>
         <v>Active</v>
       </c>
@@ -7625,7 +7612,7 @@
       <c r="D28" s="2">
         <v>5</v>
       </c>
-      <c r="E28" s="37" t="str">
+      <c r="E28" s="36" t="str">
         <f ca="1"/>
         <v>Active</v>
       </c>
@@ -7648,7 +7635,7 @@
       <c r="D29" s="2">
         <v>6</v>
       </c>
-      <c r="E29" s="37" t="e">
+      <c r="E29" s="36" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -7671,7 +7658,7 @@
       <c r="D30" s="2">
         <v>7</v>
       </c>
-      <c r="E30" s="37" t="e">
+      <c r="E30" s="36" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -7694,7 +7681,7 @@
       <c r="D31" s="2">
         <v>8</v>
       </c>
-      <c r="E31" s="37" t="e">
+      <c r="E31" s="36" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -7717,7 +7704,7 @@
       <c r="D32" s="2">
         <v>9</v>
       </c>
-      <c r="E32" s="37" t="e">
+      <c r="E32" s="36" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -7740,7 +7727,7 @@
       <c r="D33" s="2">
         <v>10</v>
       </c>
-      <c r="E33" s="37" t="e">
+      <c r="E33" s="36" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -7789,7 +7776,7 @@
   <dimension ref="B1:R32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8086,7 +8073,7 @@
         <v>202</v>
       </c>
       <c r="F21" s="33" t="str">
-        <f t="array" ref="F21:K31">_xll.flInstrumentsLookup(F19,E22:E31)</f>
+        <f t="array" ref="F21:J31">_xll.flInstrumentsLookup(F19,E22:E31)</f>
         <v>State</v>
       </c>
       <c r="G21" s="33" t="str">
@@ -8101,9 +8088,7 @@
       <c r="J21" s="33" t="str">
         <v>ClientInternal</v>
       </c>
-      <c r="K21" s="33" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
@@ -8130,12 +8115,10 @@
       <c r="I22" s="35" t="str">
         <v>BBG000B9XRY4</v>
       </c>
-      <c r="J22" s="36" t="str">
+      <c r="J22" s="52" t="str">
         <v>ExcelID1</v>
       </c>
-      <c r="K22" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
@@ -8147,7 +8130,7 @@
       <c r="D23" s="9">
         <v>2</v>
       </c>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="36" t="s">
         <v>189</v>
       </c>
       <c r="F23" s="18" t="str">
@@ -8162,12 +8145,10 @@
       <c r="I23" s="35" t="str">
         <v>BBG000DMBXR2</v>
       </c>
-      <c r="J23" s="36">
+      <c r="J23" s="52">
         <v>0</v>
       </c>
-      <c r="K23" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
@@ -8179,7 +8160,7 @@
       <c r="D24" s="9">
         <v>3</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E24" s="36" t="s">
         <v>190</v>
       </c>
       <c r="F24" s="18" t="str">
@@ -8194,12 +8175,10 @@
       <c r="I24" s="35" t="str">
         <v>BBG000C059M6</v>
       </c>
-      <c r="J24" s="36">
+      <c r="J24" s="52">
         <v>0</v>
       </c>
-      <c r="K24" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
@@ -8211,7 +8190,7 @@
       <c r="D25" s="9">
         <v>4</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="36" t="s">
         <v>191</v>
       </c>
       <c r="F25" s="18" t="str">
@@ -8226,12 +8205,10 @@
       <c r="I25" s="35" t="str">
         <v>BBG00DQ4YZ36</v>
       </c>
-      <c r="J25" s="36">
+      <c r="J25" s="52">
         <v>0</v>
       </c>
-      <c r="K25" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="P25" s="19"/>
       <c r="Q25" s="19"/>
@@ -8243,7 +8220,7 @@
       <c r="D26" s="9">
         <v>5</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="36" t="s">
         <v>192</v>
       </c>
       <c r="F26" s="18" t="str">
@@ -8258,12 +8235,10 @@
       <c r="I26" s="35" t="str">
         <v>BBG000BCM915</v>
       </c>
-      <c r="J26" s="36">
+      <c r="J26" s="52">
         <v>0</v>
       </c>
-      <c r="K26" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
@@ -8275,7 +8250,7 @@
       <c r="D27" s="9">
         <v>6</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="36" t="s">
         <v>193</v>
       </c>
       <c r="F27" s="18" t="str">
@@ -8290,12 +8265,10 @@
       <c r="I27" s="35" t="str">
         <v>BBG000BCH458</v>
       </c>
-      <c r="J27" s="36">
+      <c r="J27" s="52">
         <v>0</v>
       </c>
-      <c r="K27" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
@@ -8307,7 +8280,7 @@
       <c r="D28" s="9">
         <v>7</v>
       </c>
-      <c r="E28" s="37" t="s">
+      <c r="E28" s="36" t="s">
         <v>194</v>
       </c>
       <c r="F28" s="18" t="str">
@@ -8322,12 +8295,10 @@
       <c r="I28" s="35" t="str">
         <v>BBG000BS1MT4</v>
       </c>
-      <c r="J28" s="36">
+      <c r="J28" s="52">
         <v>0</v>
       </c>
-      <c r="K28" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="Q28" s="19"/>
       <c r="R28" s="19"/>
@@ -8338,7 +8309,7 @@
       <c r="D29" s="9">
         <v>8</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E29" s="36" t="s">
         <v>195</v>
       </c>
       <c r="F29" s="18" t="str">
@@ -8353,12 +8324,10 @@
       <c r="I29" s="35" t="str">
         <v>BBG000BH4R78</v>
       </c>
-      <c r="J29" s="36" t="str">
+      <c r="J29" s="52" t="str">
         <v>ExcelID22</v>
       </c>
-      <c r="K29" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
@@ -8367,7 +8336,7 @@
       <c r="D30" s="9">
         <v>9</v>
       </c>
-      <c r="E30" s="37" t="s">
+      <c r="E30" s="36" t="s">
         <v>196</v>
       </c>
       <c r="F30" s="18" t="str">
@@ -8382,12 +8351,10 @@
       <c r="I30" s="35" t="str">
         <v>BBG000BPH459</v>
       </c>
-      <c r="J30" s="36">
+      <c r="J30" s="52">
         <v>0</v>
       </c>
-      <c r="K30" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
@@ -8396,7 +8363,7 @@
       <c r="D31" s="9">
         <v>10</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="36" t="s">
         <v>197</v>
       </c>
       <c r="F31" s="18" t="str">
@@ -8411,12 +8378,10 @@
       <c r="I31" s="35" t="str">
         <v>BBG000CLY2D3</v>
       </c>
-      <c r="J31" s="36">
+      <c r="J31" s="52">
         <v>0</v>
       </c>
-      <c r="K31" s="36" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
@@ -8464,7 +8429,7 @@
   <dimension ref="B1:S48"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8710,7 +8675,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -8824,7 +8789,7 @@
         <v>317</v>
       </c>
       <c r="J21" s="15"/>
-      <c r="K21" s="51" t="str">
+      <c r="K21" s="50" t="str">
         <f>_xll.flInstrumentsAdd(E20:J21)</f>
         <v>LUID_RVXW0J4Z</v>
       </c>
@@ -8891,7 +8856,7 @@
         <v>317</v>
       </c>
       <c r="J24" s="15"/>
-      <c r="K24" s="51" t="str">
+      <c r="K24" s="50" t="str">
         <f>_xll.flInstrumentsAdd(E23:J24)</f>
         <v>LUID_9SBVLHHA</v>
       </c>
@@ -9122,7 +9087,7 @@
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="38"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -9262,7 +9227,7 @@
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="38"/>
+      <c r="D48" s="37"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -9309,8 +9274,8 @@
   </sheetPr>
   <dimension ref="B1:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9610,7 +9575,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="51" t="str">
+      <c r="K19" s="50" t="str">
         <f>_xll.flInstrumentsAdd(E18:J19)</f>
         <v>LUID_A9RLV8U6</v>
       </c>
@@ -9775,7 +9740,7 @@
       <c r="J29" s="17" t="str">
         <v>NewInst14</v>
       </c>
-      <c r="K29" s="51" t="str">
+      <c r="K29" s="50" t="str">
         <v>BBG007FAKECO</v>
       </c>
       <c r="L29" s="2"/>
@@ -9808,13 +9773,13 @@
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
     </row>
   </sheetData>
   <dataValidations count="18">
@@ -9853,10 +9818,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:N43"/>
+  <dimension ref="B1:N46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40:L42"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10029,8 +9994,13 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="8" t="str">
+        <f>_xll.flPropertiesAdd_Template()</f>
+        <v>OK</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -10040,29 +10010,41 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-      <c r="C13" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>287</v>
+      </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>306</v>
-      </c>
+      <c r="C14" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -10077,64 +10059,51 @@
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="L15" s="6" t="str">
-        <f t="array" ref="L15:L17">_xll.flPropertiesAdd(E15:K17)</f>
-        <v>Keys</v>
-      </c>
-      <c r="M15" s="8"/>
+      <c r="D15" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="H16" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="16" t="str">
-        <f>G16</f>
-        <v>PlanType</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="L16" s="51" t="str">
-        <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/PlanType' because it already exists.</v>
-      </c>
-      <c r="M16" s="15"/>
+      <c r="E16" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="L16" s="6" t="str">
+        <f t="array" ref="L16:L18">_xll.flPropertiesAdd(E16:K18)</f>
+        <v>Keys</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
@@ -10147,38 +10116,56 @@
         <v>296</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="H17" s="43" t="b">
+        <v>297</v>
+      </c>
+      <c r="H17" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="42" t="s">
-        <v>299</v>
-      </c>
-      <c r="J17" s="44" t="s">
-        <v>290</v>
+      <c r="I17" s="16" t="str">
+        <f>G17</f>
+        <v>PlanType</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>288</v>
       </c>
       <c r="K17" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="L17" s="51" t="str">
-        <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/TakeOverWorldDate' because it already exists.</v>
-      </c>
-      <c r="M17" s="15"/>
+      <c r="L17" s="50" t="str">
+        <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/PlanType' because it already exists.</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="15"/>
+      <c r="E18" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="H18" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>299</v>
+      </c>
+      <c r="J18" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="L18" s="50" t="str">
+        <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/TakeOverWorldDate' because it already exists.</v>
+      </c>
+      <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -10186,14 +10173,14 @@
       <c r="C19" s="2"/>
       <c r="D19" s="9"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="42"/>
+      <c r="F19" s="41"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="43"/>
       <c r="K19" s="15"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="15"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -10201,14 +10188,14 @@
       <c r="C20" s="2"/>
       <c r="D20" s="9"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="42"/>
+      <c r="F20" s="41"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="43"/>
       <c r="K20" s="15"/>
       <c r="L20" s="51"/>
-      <c r="M20" s="15"/>
+      <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -10216,14 +10203,14 @@
       <c r="C21" s="2"/>
       <c r="D21" s="9"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="42"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="44"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="43"/>
       <c r="K21" s="15"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="15"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -10231,56 +10218,57 @@
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="42"/>
+      <c r="F22" s="41"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="44"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="15"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="15"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="51"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="25" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-      <c r="C25" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="8" t="str">
+        <f>_xll.flInstrumentPropertiesAdd_Template()</f>
+        <v>OK</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -10293,55 +10281,39 @@
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="G27" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="I27" s="33" t="s">
-        <v>301</v>
-      </c>
-      <c r="J27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="6"/>
       <c r="K27" s="8"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="9">
-        <v>1</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="F28" s="15" t="str">
-        <f>'Add instrument'!K19</f>
-        <v>LUID_A9RLV8U6</v>
-      </c>
-      <c r="G28" s="47">
-        <v>43101</v>
-      </c>
-      <c r="H28" s="43" t="s">
-        <v>302</v>
-      </c>
-      <c r="I28" s="46" t="s">
-        <v>320</v>
-      </c>
-      <c r="J28" s="42"/>
-      <c r="K28" s="51" t="str">
-        <f>_xll.flInstrumentPropertiesAdd(E27:I28)</f>
-        <v>OK</v>
-      </c>
+      <c r="C28" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -10349,16 +10321,16 @@
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="9">
-        <v>2</v>
-      </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="51"/>
+      <c r="D29" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -10366,16 +10338,24 @@
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="9">
-        <v>3</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="51"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -10383,14 +10363,30 @@
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="51"/>
+      <c r="D31" s="9">
+        <v>1</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="F31" s="15" t="str">
+        <f>'Add instrument'!K19</f>
+        <v>LUID_A9RLV8U6</v>
+      </c>
+      <c r="G31" s="46">
+        <v>43101</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>302</v>
+      </c>
+      <c r="I31" s="45" t="s">
+        <v>319</v>
+      </c>
+      <c r="J31" s="41"/>
+      <c r="K31" s="50" t="str">
+        <f>_xll.flInstrumentPropertiesAdd(E30:I31)</f>
+        <v>OK</v>
+      </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -10398,14 +10394,16 @@
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="D32" s="9">
+        <v>2</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="50"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -10413,31 +10411,31 @@
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="D33" s="9">
+        <v>3</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="50"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
-      <c r="C34" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="50"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -10445,9 +10443,7 @@
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>307</v>
-      </c>
+      <c r="D35" s="9"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -10459,7 +10455,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -10474,16 +10470,14 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="C37" s="10" t="s">
+        <v>303</v>
+      </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>221</v>
-      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -10496,8 +10490,10 @@
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="9"/>
+      <c r="D38" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -10508,97 +10504,84 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F39" s="8" t="str">
-        <f t="array" ref="F39:L40">_xll.flInstrumentsLookup(F37,E40:E41,H27&amp;","&amp;I27)</f>
-        <v>State</v>
-      </c>
-      <c r="G39" s="8" t="str">
-        <v>LusidInstrumentId</v>
-      </c>
-      <c r="H39" s="8" t="str">
-        <v>Name</v>
-      </c>
-      <c r="I39" s="8" t="str">
-        <v>TakeOverDate</v>
-      </c>
-      <c r="J39" s="8" t="str">
-        <v>PlanType</v>
-      </c>
-      <c r="K39" s="8" t="str">
-        <v>Figi</v>
-      </c>
-      <c r="L39" s="8" t="str">
-        <v>ClientInternal</v>
-      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="15" t="str">
-        <f>F28</f>
-        <v>LUID_A9RLV8U6</v>
-      </c>
-      <c r="F40" s="43" t="str">
-        <v>Active</v>
-      </c>
-      <c r="G40" s="43" t="str">
-        <v>LUID_A9RLV8U6</v>
-      </c>
-      <c r="H40" s="42" t="str">
-        <v>Spectre</v>
-      </c>
-      <c r="I40" s="42" t="str">
-        <v>2028/12/01T00:00:00.00</v>
-      </c>
-      <c r="J40" s="42" t="str">
-        <v>Laser from satellite</v>
-      </c>
-      <c r="K40" s="42" t="str">
-        <v>BBG007FAKECO</v>
-      </c>
-      <c r="L40" s="51" t="str">
-        <v>NewInst14</v>
-      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="51"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="51"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="F42" s="8" t="str">
+        <f t="array" ref="F42:L43">_xll.flInstrumentsLookup(F40,E43:E44,H30&amp;","&amp;I30)</f>
+        <v>State</v>
+      </c>
+      <c r="G42" s="8" t="str">
+        <v>LusidInstrumentId</v>
+      </c>
+      <c r="H42" s="8" t="str">
+        <v>Name</v>
+      </c>
+      <c r="I42" s="8" t="str">
+        <v>TakeOverDate</v>
+      </c>
+      <c r="J42" s="8" t="str">
+        <v>PlanType</v>
+      </c>
+      <c r="K42" s="8" t="str">
+        <v>ClientInternal</v>
+      </c>
+      <c r="L42" s="8" t="str">
+        <v>Figi</v>
+      </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
@@ -10606,35 +10589,108 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="9"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+      <c r="E43" s="15" t="str">
+        <f>F31</f>
+        <v>LUID_A9RLV8U6</v>
+      </c>
+      <c r="F43" s="42" t="str">
+        <v>Active</v>
+      </c>
+      <c r="G43" s="42" t="str">
+        <v>LUID_A9RLV8U6</v>
+      </c>
+      <c r="H43" s="41" t="str">
+        <v>Spectre</v>
+      </c>
+      <c r="I43" s="41" t="str">
+        <v>2028/12/01T00:00:00.00</v>
+      </c>
+      <c r="J43" s="41" t="str">
+        <v>Laser from satellite</v>
+      </c>
+      <c r="K43" s="41" t="str">
+        <v>NewInst14</v>
+      </c>
+      <c r="L43" s="50" t="str">
+        <v>BBG007FAKECO</v>
+      </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
   </sheetData>
-  <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LifeTime" sqref="K15" xr:uid="{E7540E92-E5BE-4552-BF9C-DBFEE096FB3D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DataTypeId" sqref="J15" xr:uid="{9DF3B153-0F3B-469A-9200-5B6DE7B37C11}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DisplayName" sqref="I15" xr:uid="{B4F6905F-0F6E-454B-8D5A-DE90891032B9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ValueRequired" sqref="H15" xr:uid="{7DD8BA18-A28C-4E41-A74B-A6C2DAB47D7E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Code" sqref="G15" xr:uid="{4B063AB7-7753-4C5D-8D43-C8FF9EF43328}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scope" sqref="F15" xr:uid="{7B2DCFD6-DE2A-4DD9-91A8-A03CF34D8212}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Domain" sqref="E15" xr:uid="{D6668F53-E37A-4C9A-8F06-9EFDC70FF4B2}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="EffectiveFrom" sqref="Q16" xr:uid="{24A97234-1260-44ED-B57D-A9A5CDFE549A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="SecurityUid" sqref="P16" xr:uid="{98DF1528-AB19-418D-8363-FCCF64C101A6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique Lusid Instrument Identifier (LUID) of the instrument to update or insert properties on." sqref="L32 O33" xr:uid="{5F7002E7-75EE-451D-8512-06F52438E5BA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The effective datetime from which the property is valid" sqref="M32 P33" xr:uid="{5461AD21-5889-4A6D-9EF8-C2F9E2313963}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Replace this with your custom properties; here and in the columns to the right [Set of unique instrument properties and associated values to store with the instrument. Each property must be from the 'Instrument' domain.]" sqref="N32 Q33" xr:uid="{2A9A010A-6017-49BD-AEE0-081D3CADD4D4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The instrument identifier type." sqref="E33" xr:uid="{4374EB16-DCB5-4C88-87AB-2DEDE8518DD5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique instrument identifier of the instrument to update or insert properties on." sqref="F33" xr:uid="{4CC13194-FA28-4F34-A9A8-89FE1E4D6517}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The effective datetime from which the property is valid" sqref="G33" xr:uid="{3DCACC70-6565-46CC-B179-11E4D4ADB398}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Replace this with your custom properties; here and in the columns to the right [Set of unique instrument properties and associated values to store with the instrument. Each property must be from the 'Instrument' domain.]" sqref="H33" xr:uid="{D7729818-3906-4D67-A751-4600C40FD1E4}"/>
+  <dataValidations count="27">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LifeTime" sqref="K16" xr:uid="{E7540E92-E5BE-4552-BF9C-DBFEE096FB3D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DataTypeId" sqref="J16" xr:uid="{9DF3B153-0F3B-469A-9200-5B6DE7B37C11}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DisplayName" sqref="I16" xr:uid="{B4F6905F-0F6E-454B-8D5A-DE90891032B9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ValueRequired" sqref="H16" xr:uid="{7DD8BA18-A28C-4E41-A74B-A6C2DAB47D7E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Code" sqref="G16" xr:uid="{4B063AB7-7753-4C5D-8D43-C8FF9EF43328}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scope" sqref="F16" xr:uid="{7B2DCFD6-DE2A-4DD9-91A8-A03CF34D8212}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Domain" sqref="E16" xr:uid="{D6668F53-E37A-4C9A-8F06-9EFDC70FF4B2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="EffectiveFrom" sqref="Q17" xr:uid="{24A97234-1260-44ED-B57D-A9A5CDFE549A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="SecurityUid" sqref="P17" xr:uid="{98DF1528-AB19-418D-8363-FCCF64C101A6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique Lusid Instrument Identifier (LUID) of the instrument to update or insert properties on." sqref="L35 O36" xr:uid="{5F7002E7-75EE-451D-8512-06F52438E5BA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The effective datetime from which the property is valid" sqref="M35 P36 G36" xr:uid="{5461AD21-5889-4A6D-9EF8-C2F9E2313963}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Replace this with your custom properties; here and in the columns to the right [Set of unique instrument properties and associated values to store with the instrument. Each property must be from the 'Instrument' domain.]" sqref="N35 Q36 H36" xr:uid="{2A9A010A-6017-49BD-AEE0-081D3CADD4D4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The instrument identifier type." sqref="E36" xr:uid="{4374EB16-DCB5-4C88-87AB-2DEDE8518DD5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique instrument identifier of the instrument to update or insert properties on." sqref="F36" xr:uid="{4CC13194-FA28-4F34-A9A8-89FE1E4D6517}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The content of the expanded definition. There is no validation on the format of this." sqref="J27" xr:uid="{B17764F2-0C34-422E-BE14-227E429FB3CB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format of the expanded definition." sqref="I27" xr:uid="{82F01F84-21EF-4F43-A9D7-A6A394AE18BB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The instrument identifier type." sqref="E27" xr:uid="{C58E0E4E-4CE0-408E-8ACE-90D2FD3DAAF0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique instrument identifier of the instrument to update or insert properties on." sqref="F27" xr:uid="{7AD6046B-EABB-4A6B-A667-50450DD3207D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The effective datetime from which the property is valid" sqref="G27" xr:uid="{02E2C89D-A54E-4478-AD8E-E1609667735A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Replace this with your custom properties; here and in the columns to the right [Set of unique instrument properties and associated values to store with the instrument. Each property must be from the 'Instrument' domain.]" sqref="H27" xr:uid="{38C3D282-32C5-47B2-8F8A-DD0114CD64DC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Domain" sqref="E13" xr:uid="{D52AB31C-C372-4BA4-9B91-60ED7BE937D9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scope" sqref="F13" xr:uid="{E17E1A74-67FD-4259-AA6D-43A4F125D65F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Code" sqref="G13" xr:uid="{F8387888-3242-4EBF-B814-3CEC89BA1939}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ValueRequired" sqref="H13" xr:uid="{5A37A396-448B-4925-B797-2084F8FDA6FC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DisplayName" sqref="I13" xr:uid="{B2D0A61E-A1EF-475D-8099-E5572A527286}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DataTypeId" sqref="J13" xr:uid="{EA368FFF-F58E-4FBB-9234-06D15EB562AB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LifeTime" sqref="K13" xr:uid="{E37AADCD-69AA-46EB-8FFD-1C620AF704DA}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E8" r:id="rId1" xr:uid="{D5E1FEFA-AE04-4FB3-8E4A-D3598E42A3B1}"/>
@@ -10655,7 +10711,7 @@
   <dimension ref="B1:V37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22:N30"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11128,7 +11184,7 @@
       </c>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="52">
+      <c r="N22" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E22,G22,H22,I22,J22,K22,L22,M22)</f>
         <v>100</v>
       </c>
@@ -11167,7 +11223,7 @@
       </c>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
-      <c r="N23" s="52">
+      <c r="N23" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E23,G23,H23,I23,J23,K23,L23,M23)</f>
         <v>199.25</v>
       </c>
@@ -11206,7 +11262,7 @@
       </c>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
-      <c r="N24" s="52">
+      <c r="N24" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E24,G24,H24,I24,J24,K24,L24,M24)</f>
         <v>203.13</v>
       </c>
@@ -11245,7 +11301,7 @@
       </c>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
-      <c r="N25" s="52">
+      <c r="N25" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E25,G25,H25,I25,J25,K25,L25,M25)</f>
         <v>203.86</v>
       </c>
@@ -11284,7 +11340,7 @@
       </c>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
-      <c r="N26" s="52">
+      <c r="N26" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E26,G26,H26,I26,J26,K26,L26,M26)</f>
         <v>203.86</v>
       </c>
@@ -11320,7 +11376,7 @@
       </c>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
-      <c r="N27" s="52">
+      <c r="N27" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E27,G27,H27,I27,J27,K27,L27,M27)</f>
         <v>203.86</v>
       </c>
@@ -11356,7 +11412,7 @@
       </c>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
-      <c r="N28" s="52">
+      <c r="N28" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E28,G28,H28,I28,J28,K28,L28,M28)</f>
         <v>203.86</v>
       </c>
@@ -11392,7 +11448,7 @@
       </c>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
-      <c r="N29" s="52">
+      <c r="N29" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E29,G29,H29,I29,J29,K29,L29,M29)</f>
         <v>204.53</v>
       </c>
@@ -11428,7 +11484,7 @@
       </c>
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
-      <c r="N30" s="52">
+      <c r="N30" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E30,G30,H30,I30,J30,K30,L30,M30)</f>
         <v>207.48</v>
       </c>
@@ -11897,7 +11953,7 @@
         <v>43570</v>
       </c>
       <c r="L22" s="20"/>
-      <c r="M22" s="52">
+      <c r="M22" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E22,G22,H22,I22,J22,K22,F22,L22)</f>
         <v>100</v>
       </c>
@@ -11930,7 +11986,7 @@
         <v>43571</v>
       </c>
       <c r="L23" s="17"/>
-      <c r="M23" s="52">
+      <c r="M23" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E23,G23,H23,I23,J23,K23,F23,L23)</f>
         <v>111.1</v>
       </c>
@@ -11963,7 +12019,7 @@
         <v>43572</v>
       </c>
       <c r="L24" s="17"/>
-      <c r="M24" s="52">
+      <c r="M24" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E24,G24,H24,I24,J24,K24,F24,L24)</f>
         <v>78.36</v>
       </c>
@@ -11996,7 +12052,7 @@
         <v>43573</v>
       </c>
       <c r="L25" s="17"/>
-      <c r="M25" s="52">
+      <c r="M25" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E25,G25,H25,I25,J25,K25,F25,L25)</f>
         <v>166.6</v>
       </c>
@@ -12030,7 +12086,7 @@
         <v>43574</v>
       </c>
       <c r="L26" s="17"/>
-      <c r="M26" s="52">
+      <c r="M26" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E26,G26,H26,I26,J26,K26,F26,L26)</f>
         <v>666.5</v>
       </c>
@@ -12061,7 +12117,7 @@
         <v>43575</v>
       </c>
       <c r="L27" s="17"/>
-      <c r="M27" s="52">
+      <c r="M27" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E27,G27,H27,I27,J27,K27,F27,L27)</f>
         <v>132.44999999999999</v>
       </c>
@@ -12092,7 +12148,7 @@
         <v>43576</v>
       </c>
       <c r="L28" s="17"/>
-      <c r="M28" s="52">
+      <c r="M28" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E28,G28,H28,I28,J28,K28,F28,L28)</f>
         <v>123.37</v>
       </c>
@@ -12123,7 +12179,7 @@
         <v>43577</v>
       </c>
       <c r="L29" s="17"/>
-      <c r="M29" s="52">
+      <c r="M29" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E29,G29,H29,I29,J29,K29,F29,L29)</f>
         <v>6963</v>
       </c>
@@ -12154,7 +12210,7 @@
         <v>43578</v>
       </c>
       <c r="L30" s="17"/>
-      <c r="M30" s="52">
+      <c r="M30" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E30,G30,H30,I30,J30,K30,F30,L30)</f>
         <v>582.5</v>
       </c>
@@ -12185,7 +12241,7 @@
         <v>43579</v>
       </c>
       <c r="L31" s="17"/>
-      <c r="M31" s="52">
+      <c r="M31" s="51">
         <f>_xll.flQuoteGetForDate($F$15,E31,G31,H31,I31,J31,K31,F31,L31)</f>
         <v>11550</v>
       </c>
@@ -12453,6 +12509,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -12460,15 +12525,6 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12492,9 +12548,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F07F7B26-A8FB-44CC-BC1A-494CF9683469}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -12503,16 +12566,9 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
     <ds:schemaRef ds:uri="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DEV-6025 completed fixes for changing param lists
</commit_message>
<xml_diff>
--- a/LUSID Excel - Setting up your market data.xlsx
+++ b/LUSID Excel - Setting up your market data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusSekhon\Dev\sample-excel\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445D62FA-1A9F-41EC-9D3C-AF9FC39F8181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FFC1CE-CA95-4937-AB06-E20B7FB6F6ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" firstSheet="1" activeTab="10" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Datetime format" sheetId="21" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="345">
   <si>
     <t>Base Currency</t>
   </si>
@@ -777,9 +777,6 @@
     <t>Figi</t>
   </si>
   <si>
-    <t>Mid</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scope: </t>
   </si>
   <si>
@@ -1195,6 +1192,9 @@
   </si>
   <si>
     <t>BBG007FAKECO</t>
+  </si>
+  <si>
+    <t>mid</t>
   </si>
 </sst>
 </file>
@@ -1530,364 +1530,371 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>e33b658a-70cf-4d5b-a585-87d33bd850dd</stp>
-        <tr r="H26" s="10"/>
-        <tr r="F28" s="10"/>
-        <tr r="G31" s="10"/>
-        <tr r="I28" s="10"/>
-        <tr r="F22" s="10"/>
-        <tr r="I25" s="10"/>
-        <tr r="F31" s="10"/>
-        <tr r="F26" s="10"/>
-        <tr r="G24" s="10"/>
-        <tr r="I26" s="10"/>
-        <tr r="I24" s="10"/>
-        <tr r="I22" s="10"/>
-        <tr r="H23" s="10"/>
-        <tr r="F27" s="10"/>
-        <tr r="J21" s="10"/>
-        <tr r="J30" s="10"/>
-        <tr r="I30" s="10"/>
-        <tr r="G22" s="10"/>
-        <tr r="G21" s="10"/>
-        <tr r="G23" s="10"/>
-        <tr r="I31" s="10"/>
-        <tr r="J28" s="10"/>
-        <tr r="F29" s="10"/>
-        <tr r="J31" s="10"/>
-        <tr r="G29" s="10"/>
-        <tr r="I21" s="10"/>
-        <tr r="G27" s="10"/>
-        <tr r="G26" s="10"/>
-        <tr r="F30" s="10"/>
-        <tr r="J27" s="10"/>
-        <tr r="H29" s="10"/>
-        <tr r="H31" s="10"/>
-        <tr r="H24" s="10"/>
-        <tr r="H30" s="10"/>
-        <tr r="F24" s="10"/>
-        <tr r="H28" s="10"/>
-        <tr r="H25" s="10"/>
-        <tr r="J26" s="10"/>
-        <tr r="I23" s="10"/>
-        <tr r="G25" s="10"/>
-        <tr r="F23" s="10"/>
-        <tr r="I29" s="10"/>
-        <tr r="H22" s="10"/>
-        <tr r="H27" s="10"/>
-        <tr r="J22" s="10"/>
-        <tr r="I27" s="10"/>
-        <tr r="G28" s="10"/>
-        <tr r="J24" s="10"/>
-        <tr r="J25" s="10"/>
-        <tr r="G30" s="10"/>
-        <tr r="F25" s="10"/>
-        <tr r="J23" s="10"/>
-        <tr r="H21" s="10"/>
-        <tr r="J29" s="10"/>
-        <tr r="F21" s="10"/>
+        <stp>9c58753e-ee55-431c-bc50-24f145f51a03</stp>
+        <tr r="M23" s="17"/>
       </tp>
     </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>dda1fa4d-a546-4508-a1bb-09c7c78f8964</stp>
-        <tr r="N29" s="16"/>
+        <stp>50b35d4b-128c-497b-ae21-079eb40bb2dd</stp>
+        <tr r="N25" s="16"/>
       </tp>
     </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>b2552618-2b29-45a5-bd89-61e7efd8fd32</stp>
-        <tr r="F43" s="20"/>
-        <tr r="L43" s="20"/>
-        <tr r="I43" s="20"/>
-        <tr r="G42" s="20"/>
-        <tr r="H42" s="20"/>
-        <tr r="I42" s="20"/>
-        <tr r="J43" s="20"/>
-        <tr r="L42" s="20"/>
-        <tr r="H43" s="20"/>
-        <tr r="J42" s="20"/>
-        <tr r="K42" s="20"/>
-        <tr r="F42" s="20"/>
-        <tr r="G43" s="20"/>
-        <tr r="K43" s="20"/>
+        <stp>11165e86-7c93-4b5c-b92b-1766822d54a1</stp>
+        <tr r="H26" s="10"/>
+        <tr r="G24" s="10"/>
+        <tr r="I30" s="10"/>
+        <tr r="G29" s="10"/>
+        <tr r="H24" s="10"/>
+        <tr r="F23" s="10"/>
+        <tr r="J25" s="10"/>
+        <tr r="F28" s="10"/>
+        <tr r="I26" s="10"/>
+        <tr r="G22" s="10"/>
+        <tr r="I21" s="10"/>
+        <tr r="H30" s="10"/>
+        <tr r="I29" s="10"/>
+        <tr r="G30" s="10"/>
+        <tr r="G31" s="10"/>
+        <tr r="I24" s="10"/>
+        <tr r="G21" s="10"/>
+        <tr r="G27" s="10"/>
+        <tr r="F24" s="10"/>
+        <tr r="H22" s="10"/>
+        <tr r="F25" s="10"/>
+        <tr r="I28" s="10"/>
+        <tr r="I22" s="10"/>
+        <tr r="G23" s="10"/>
+        <tr r="G26" s="10"/>
+        <tr r="H28" s="10"/>
+        <tr r="H27" s="10"/>
+        <tr r="J23" s="10"/>
+        <tr r="F22" s="10"/>
+        <tr r="H23" s="10"/>
+        <tr r="I31" s="10"/>
+        <tr r="F30" s="10"/>
+        <tr r="H25" s="10"/>
+        <tr r="J22" s="10"/>
+        <tr r="H21" s="10"/>
+        <tr r="I25" s="10"/>
+        <tr r="F27" s="10"/>
+        <tr r="J28" s="10"/>
+        <tr r="J27" s="10"/>
+        <tr r="J26" s="10"/>
+        <tr r="I27" s="10"/>
+        <tr r="J29" s="10"/>
+        <tr r="F31" s="10"/>
+        <tr r="J21" s="10"/>
+        <tr r="F29" s="10"/>
+        <tr r="H29" s="10"/>
+        <tr r="I23" s="10"/>
+        <tr r="G28" s="10"/>
+        <tr r="F21" s="10"/>
+        <tr r="F26" s="10"/>
+        <tr r="J30" s="10"/>
+        <tr r="J31" s="10"/>
+        <tr r="H31" s="10"/>
+        <tr r="G25" s="10"/>
+        <tr r="J24" s="10"/>
       </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>4afcd1e3-b73e-41e8-82a8-f2b303e64ae0</stp>
-        <tr r="G25" s="11"/>
-        <tr r="F19" s="11"/>
-        <tr r="E23" s="11"/>
-        <tr r="E20" s="11"/>
-        <tr r="E22" s="11"/>
-        <tr r="E28" s="11"/>
-        <tr r="F27" s="11"/>
-        <tr r="F28" s="11"/>
-        <tr r="F20" s="11"/>
-        <tr r="G29" s="11"/>
-        <tr r="G19" s="11"/>
-        <tr r="G22" s="11"/>
-        <tr r="G20" s="11"/>
-        <tr r="E26" s="11"/>
-        <tr r="F17" s="11"/>
-        <tr r="F18" s="11"/>
-        <tr r="G23" s="11"/>
-        <tr r="F21" s="11"/>
-        <tr r="F24" s="11"/>
-        <tr r="E17" s="11"/>
-        <tr r="E29" s="11"/>
-        <tr r="E24" s="11"/>
-        <tr r="F26" s="11"/>
-        <tr r="G24" s="11"/>
-        <tr r="E25" s="11"/>
-        <tr r="G28" s="11"/>
-        <tr r="G26" s="11"/>
-        <tr r="F29" s="11"/>
-        <tr r="E19" s="11"/>
-        <tr r="G27" s="11"/>
-        <tr r="E18" s="11"/>
-        <tr r="E21" s="11"/>
-        <tr r="G17" s="11"/>
-        <tr r="F23" s="11"/>
-        <tr r="F25" s="11"/>
-        <tr r="G18" s="11"/>
-        <tr r="G21" s="11"/>
-        <tr r="F22" s="11"/>
-        <tr r="E27" s="11"/>
+        <stp>56155feb-ba1d-4596-a41d-94f46d127f5d</stp>
+        <tr r="N24" s="16"/>
       </tp>
     </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>b790a6e4-9ea1-4eab-8863-e50dfd86a895</stp>
-        <tr r="M29" s="17"/>
+        <stp>10e5e319-55db-4ef0-b5b8-71c55264fef4</stp>
+        <tr r="J42" s="20"/>
+        <tr r="J43" s="20"/>
+        <tr r="I42" s="20"/>
+        <tr r="F43" s="20"/>
+        <tr r="K43" s="20"/>
+        <tr r="H42" s="20"/>
+        <tr r="L42" s="20"/>
+        <tr r="I43" s="20"/>
+        <tr r="L43" s="20"/>
+        <tr r="K42" s="20"/>
+        <tr r="H43" s="20"/>
+        <tr r="G42" s="20"/>
+        <tr r="G43" s="20"/>
+        <tr r="F42" s="20"/>
       </tp>
     </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>9b2bb666-0a64-482c-8c19-dc703cd797d4</stp>
-        <tr r="N26" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>aff45025-cfb2-417a-a894-e9f102138f05</stp>
-        <tr r="N24" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>bcbbe081-7d49-4bc3-b94a-9d7ac27016f2</stp>
-        <tr r="I28" s="14"/>
-        <tr r="I29" s="14"/>
-        <tr r="K28" s="14"/>
-        <tr r="L28" s="14"/>
-        <tr r="L29" s="14"/>
-        <tr r="H28" s="14"/>
-        <tr r="G28" s="14"/>
-        <tr r="J29" s="14"/>
-        <tr r="K29" s="14"/>
-        <tr r="G29" s="14"/>
-        <tr r="H29" s="14"/>
-        <tr r="J28" s="14"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>0e4e69d4-96d2-4315-86e0-1f32970b7960</stp>
-        <tr r="M30" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>18a23769-bbad-46dc-b5be-4655e7d7b057</stp>
-        <tr r="N25" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>29a8c027-0f0d-462b-886e-ee7f5dcdd0b8</stp>
-        <tr r="M25" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>d8ecb491-5dad-43b6-bc58-a5cebd83b59d</stp>
-        <tr r="M28" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>780ef6dd-86df-4df1-96d9-49a2de7bbfe0</stp>
-        <tr r="E23" s="12"/>
-        <tr r="F23" s="12"/>
-        <tr r="E32" s="12"/>
-        <tr r="E33" s="12"/>
-        <tr r="G24" s="12"/>
-        <tr r="E29" s="12"/>
-        <tr r="G27" s="12"/>
-        <tr r="F32" s="12"/>
-        <tr r="F29" s="12"/>
-        <tr r="G30" s="12"/>
-        <tr r="E24" s="12"/>
-        <tr r="E28" s="12"/>
-        <tr r="G33" s="12"/>
-        <tr r="G29" s="12"/>
-        <tr r="G25" s="12"/>
-        <tr r="G28" s="12"/>
-        <tr r="G26" s="12"/>
-        <tr r="F27" s="12"/>
-        <tr r="F24" s="12"/>
-        <tr r="F30" s="12"/>
-        <tr r="E30" s="12"/>
-        <tr r="F31" s="12"/>
-        <tr r="G23" s="12"/>
-        <tr r="F26" s="12"/>
-        <tr r="F25" s="12"/>
-        <tr r="F28" s="12"/>
-        <tr r="E26" s="12"/>
-        <tr r="E25" s="12"/>
-        <tr r="F33" s="12"/>
-        <tr r="G32" s="12"/>
-        <tr r="E27" s="12"/>
-        <tr r="E31" s="12"/>
-        <tr r="G31" s="12"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>832c58fa-bd86-46c6-b87b-06306299d4a3</stp>
-        <tr r="N30" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>f7498c14-cc42-4591-ba33-531f28b5dd0c</stp>
-        <tr r="N28" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>a38e6fb0-8db8-4e39-941b-a4ebdf1abbcf</stp>
-        <tr r="M24" s="17"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>2554ffcc-f379-4e90-a145-0c0d55cf9298</stp>
-        <tr r="N27" s="16"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>39a96072-66d6-4982-b332-39dc8540feeb</stp>
+        <stp>1ca87041-1cfb-4cd6-b637-b23a3a2bf5c8</stp>
         <tr r="M27" s="17"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>131692bd-9d1e-4279-bbca-5a4f90d8edbc</stp>
-        <tr r="M26" s="17"/>
+        <stp>4564e3bb-89a7-416d-994c-4e1ba39698b9</stp>
+        <tr r="E28" s="11"/>
+        <tr r="G24" s="11"/>
+        <tr r="G25" s="11"/>
+        <tr r="F20" s="11"/>
+        <tr r="G23" s="11"/>
+        <tr r="E25" s="11"/>
+        <tr r="G17" s="11"/>
+        <tr r="F19" s="11"/>
+        <tr r="G29" s="11"/>
+        <tr r="F21" s="11"/>
+        <tr r="G28" s="11"/>
+        <tr r="F23" s="11"/>
+        <tr r="E21" s="11"/>
+        <tr r="E23" s="11"/>
+        <tr r="G26" s="11"/>
+        <tr r="E20" s="11"/>
+        <tr r="G22" s="11"/>
+        <tr r="E17" s="11"/>
+        <tr r="F29" s="11"/>
+        <tr r="G18" s="11"/>
+        <tr r="F28" s="11"/>
+        <tr r="F18" s="11"/>
+        <tr r="G19" s="11"/>
+        <tr r="F24" s="11"/>
+        <tr r="F25" s="11"/>
+        <tr r="E22" s="11"/>
+        <tr r="G20" s="11"/>
+        <tr r="E29" s="11"/>
+        <tr r="E19" s="11"/>
+        <tr r="G21" s="11"/>
+        <tr r="E26" s="11"/>
+        <tr r="E24" s="11"/>
+        <tr r="G27" s="11"/>
+        <tr r="F22" s="11"/>
+        <tr r="F27" s="11"/>
+        <tr r="F17" s="11"/>
+        <tr r="F26" s="11"/>
+        <tr r="E18" s="11"/>
+        <tr r="E27" s="11"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>82ae3128-2a5e-43ee-b3f4-f0a5042d4a19</stp>
+        <stp>660ce0c5-0169-4e77-9fa0-33f5bf05d52b</stp>
+        <tr r="N29" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>61a72f8a-8ffe-4f30-a9b7-836981e231d9</stp>
+        <tr r="G34" s="13"/>
+        <tr r="I36" s="13"/>
+        <tr r="H36" s="13"/>
+        <tr r="I35" s="13"/>
+        <tr r="F36" s="13"/>
+        <tr r="K36" s="13"/>
+        <tr r="G35" s="13"/>
+        <tr r="J36" s="13"/>
+        <tr r="H34" s="13"/>
+        <tr r="K34" s="13"/>
+        <tr r="H35" s="13"/>
+        <tr r="F35" s="13"/>
+        <tr r="F34" s="13"/>
+        <tr r="J35" s="13"/>
         <tr r="G36" s="13"/>
         <tr r="J34" s="13"/>
         <tr r="I34" s="13"/>
-        <tr r="G35" s="13"/>
-        <tr r="I36" s="13"/>
-        <tr r="H36" s="13"/>
-        <tr r="H34" s="13"/>
-        <tr r="I35" s="13"/>
-        <tr r="K34" s="13"/>
-        <tr r="H35" s="13"/>
         <tr r="K35" s="13"/>
-        <tr r="F34" s="13"/>
-        <tr r="J36" s="13"/>
-        <tr r="J35" s="13"/>
-        <tr r="G34" s="13"/>
-        <tr r="F36" s="13"/>
-        <tr r="K36" s="13"/>
-        <tr r="F35" s="13"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>d5e958b0-0550-4cd2-9fc4-a9186c66aaa6</stp>
+        <stp>ff50d9be-8796-46cf-809c-61c9412c7478</stp>
+        <tr r="N23" s="16"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>14023d12-416e-49cf-9df2-55334d6cf913</stp>
+        <tr r="G32" s="14"/>
+        <tr r="J33" s="14"/>
+        <tr r="L32" s="14"/>
+        <tr r="K32" s="14"/>
+        <tr r="H33" s="14"/>
+        <tr r="L33" s="14"/>
+        <tr r="G33" s="14"/>
+        <tr r="J32" s="14"/>
+        <tr r="I33" s="14"/>
+        <tr r="K33" s="14"/>
+        <tr r="I32" s="14"/>
+        <tr r="H32" s="14"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>f6fee0f4-bc85-448a-8fd6-bc8471611814</stp>
+        <tr r="N27" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>b277a61a-67f2-491e-a8fc-4929196ea86d</stp>
+        <tr r="N26" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>41f95d4e-098d-4ff3-9d2c-3506fd4b6b02</stp>
+        <tr r="M28" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>52bb8e15-0bca-4d46-a9e1-40c4fc50e3db</stp>
         <tr r="M22" s="17"/>
         <tr r="N22" s="16"/>
       </tp>
     </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>1addcb2f-7372-4280-88b1-9a20249e1bda</stp>
-        <tr r="M31" s="17"/>
+        <stp>9a339039-083f-4dbc-9488-cb2af9e842e2</stp>
+        <tr r="G31" s="14"/>
       </tp>
-    </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>9e8ec426-bebe-4960-b842-8bfb971bd2c2</stp>
-        <tr r="G31" s="14"/>
+        <stp>3f89804c-f833-451d-86ae-079bdb523285</stp>
+        <tr r="N28" s="16"/>
       </tp>
     </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>532dc68a-d3b6-4641-b10f-64ebf58ae289</stp>
-        <tr r="N23" s="16"/>
+        <stp>b9ad75ad-4b4f-4eda-9fce-7945bbc6a14b</stp>
+        <tr r="M24" s="17"/>
       </tp>
     </main>
-    <main first="rtdsrv.e1fe7aaab8fa4ccebcac0abf432fa1f9">
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>aa333e50-389a-49bc-a4cd-eec2a8e2b84a</stp>
-        <tr r="M23" s="17"/>
+        <stp>0f8f61c8-c051-41b3-b230-925142abdd92</stp>
+        <tr r="M26" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>bd9bf7cf-40da-4972-9975-ba101e1cb9e8</stp>
+        <tr r="H28" s="14"/>
+        <tr r="I29" s="14"/>
+        <tr r="K28" s="14"/>
+        <tr r="G28" s="14"/>
+        <tr r="L28" s="14"/>
+        <tr r="I28" s="14"/>
+        <tr r="J29" s="14"/>
+        <tr r="L29" s="14"/>
+        <tr r="H29" s="14"/>
+        <tr r="J28" s="14"/>
+        <tr r="G29" s="14"/>
+        <tr r="K29" s="14"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>0193442e-14bb-43c2-9db1-f13cc82ad37f</stp>
+        <tr r="N30" s="16"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>58e2aceb-df0b-4d23-bace-2a5b664d1f57</stp>
+        <tr r="M29" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>792a52a0-2195-4176-8b26-4f0bb6fab0d2</stp>
+        <tr r="F32" s="12"/>
+        <tr r="F26" s="12"/>
+        <tr r="F29" s="12"/>
+        <tr r="G31" s="12"/>
+        <tr r="F27" s="12"/>
+        <tr r="E32" s="12"/>
+        <tr r="E26" s="12"/>
+        <tr r="E33" s="12"/>
+        <tr r="E28" s="12"/>
+        <tr r="F30" s="12"/>
+        <tr r="E25" s="12"/>
+        <tr r="E31" s="12"/>
+        <tr r="G26" s="12"/>
+        <tr r="F23" s="12"/>
+        <tr r="F28" s="12"/>
+        <tr r="E24" s="12"/>
+        <tr r="G24" s="12"/>
+        <tr r="E30" s="12"/>
+        <tr r="E29" s="12"/>
+        <tr r="G29" s="12"/>
+        <tr r="F31" s="12"/>
+        <tr r="G32" s="12"/>
+        <tr r="G28" s="12"/>
+        <tr r="E23" s="12"/>
+        <tr r="F25" s="12"/>
+        <tr r="G30" s="12"/>
+        <tr r="F24" s="12"/>
+        <tr r="G33" s="12"/>
+        <tr r="F33" s="12"/>
+        <tr r="G27" s="12"/>
+        <tr r="G25" s="12"/>
+        <tr r="G23" s="12"/>
+        <tr r="E27" s="12"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>6d0dca38-6a98-4b85-9b63-aef7e9afb695</stp>
+        <tr r="M30" s="17"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bc6abdde865a49fc94a43222412530fe">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>f3cf562f-667e-474c-b027-4588f991f62c</stp>
+        <tr r="M25" s="17"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>d75cdde3-3501-4cf9-9646-55d03a2c1a7e</stp>
+        <tr r="M31" s="17"/>
       </tp>
     </main>
   </volType>
@@ -2955,8 +2962,8 @@
   </sheetPr>
   <dimension ref="B1:T31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,7 +3010,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3037,7 +3044,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3055,7 +3062,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -3074,7 +3081,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -3092,7 +3099,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -3110,7 +3117,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3144,12 +3151,12 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -3180,12 +3187,12 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -3218,20 +3225,20 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F17" s="25">
         <v>43565</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I17" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -3262,7 +3269,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F19" s="28">
         <f>F17</f>
@@ -3270,7 +3277,7 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I19" s="25" t="str">
         <f>TEXT(F23,"yyyy-mm-dd")&amp;"T"&amp;TEXT(F23," hh:mm:ss.00Z")</f>
@@ -3306,17 +3313,17 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F21" s="29">
         <v>0.56302719907407406</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="I21" s="25" t="s">
         <v>325</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>326</v>
       </c>
       <c r="J21" s="49"/>
       <c r="K21" s="2"/>
@@ -3348,7 +3355,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F23" s="30">
         <f>F17 + F21</f>
@@ -3356,7 +3363,7 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I23" s="25" t="str">
         <f>TEXT(F23,"yyyy-mm-dd")&amp;"NSingaporeClose"</f>
@@ -3390,7 +3397,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F25" s="31">
         <f>F23</f>
@@ -3427,7 +3434,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F27" s="30">
         <f>F23+1/24</f>
@@ -3464,7 +3471,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F29" s="30">
         <f>F27-1/1440</f>
@@ -3531,7 +3538,9 @@
   </sheetPr>
   <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3579,7 +3588,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3617,7 +3626,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3637,7 +3646,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -3658,7 +3667,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -3678,7 +3687,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -3698,7 +3707,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3772,7 +3781,7 @@
     <row r="13" spans="2:22" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="2"/>
@@ -3825,7 +3834,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -3931,7 +3940,7 @@
     <row r="19" spans="2:30" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -4036,22 +4045,22 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="G22" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>209</v>
-      </c>
       <c r="I22" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>187</v>
@@ -4060,16 +4069,16 @@
         <v>185</v>
       </c>
       <c r="M22" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="O22" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="N22" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="O22" s="6" t="s">
+      <c r="P22" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22"/>
@@ -4091,10 +4100,10 @@
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
       <c r="E23" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>204</v>
@@ -4106,7 +4115,7 @@
         <v>186</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K23" s="17">
         <v>100</v>
@@ -4121,7 +4130,7 @@
       <c r="O23" s="32"/>
       <c r="P23" s="50" t="str">
         <f>_xll.flQuotesAdd(F15,E22:O23)</f>
-        <v>Added 1 quote(s) as at time 2019-12-04 10:30:48Z</v>
+        <v>Added 1 quote(s) as at time 2020-01-03 14:13:07Z</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23"/>
@@ -4800,7 +4809,9 @@
   </sheetPr>
   <dimension ref="B1:Y43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4846,7 +4857,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4884,7 +4895,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4904,7 +4915,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4925,7 +4936,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -4945,7 +4956,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -4965,7 +4976,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -5027,7 +5038,7 @@
     <row r="13" spans="2:25" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="2"/>
@@ -5086,7 +5097,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -5185,7 +5196,7 @@
     <row r="19" spans="2:25" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -5233,7 +5244,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -5295,22 +5306,22 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>209</v>
-      </c>
       <c r="I23" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="J23" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>187</v>
@@ -5319,16 +5330,16 @@
         <v>185</v>
       </c>
       <c r="M23" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="O23" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="N23" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="O23" s="6" t="s">
+      <c r="P23" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23"/>
@@ -5345,22 +5356,22 @@
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>186</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K24" s="17">
         <v>1.3</v>
@@ -5375,7 +5386,7 @@
       <c r="O24" s="32"/>
       <c r="P24" s="50" t="str">
         <f>_xll.flQuotesAdd(F15,E23:O27)</f>
-        <v>Added 4 quote(s) as at time 2019-12-04 10:30:48Z</v>
+        <v>Added 4 quote(s) as at time 2020-01-03 14:13:07Z</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24"/>
@@ -5392,22 +5403,22 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
       <c r="E25" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I25" s="16" t="s">
         <v>186</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K25" s="17">
         <v>1.29</v>
@@ -5437,22 +5448,22 @@
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
       <c r="E26" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I26" s="16" t="s">
         <v>186</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K26" s="17">
         <v>1.28</v>
@@ -5482,22 +5493,22 @@
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
       <c r="E27" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I27" s="16" t="s">
         <v>186</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K27" s="17">
         <v>1.27</v>
@@ -6687,7 +6698,7 @@
   <dimension ref="B1:R30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6732,7 +6743,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -6760,7 +6771,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -6775,7 +6786,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -6791,7 +6802,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -6806,7 +6817,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -6821,7 +6832,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -6878,7 +6889,7 @@
     <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -6979,13 +6990,13 @@
       <c r="C19" s="2"/>
       <c r="D19" s="9"/>
       <c r="E19" s="36" t="str">
-        <v>CompositeFigi</v>
+        <v>EdiKey</v>
       </c>
       <c r="F19" s="18" t="str">
-        <v>Instrument/default/CompositeFigi</v>
+        <v>Instrument/default/EdiKey</v>
       </c>
       <c r="G19" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -7001,10 +7012,10 @@
       <c r="C20" s="2"/>
       <c r="D20" s="9"/>
       <c r="E20" s="36" t="str">
-        <v>Ticker</v>
+        <v>ShareClassFigi</v>
       </c>
       <c r="F20" s="18" t="str">
-        <v>Instrument/default/Ticker</v>
+        <v>Instrument/default/ShareClassFigi</v>
       </c>
       <c r="G20" s="18" t="b">
         <v>0</v>
@@ -7045,10 +7056,10 @@
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
       <c r="E22" s="36" t="str">
-        <v>Cusip</v>
+        <v>Ticker</v>
       </c>
       <c r="F22" s="18" t="str">
-        <v>Instrument/default/Cusip</v>
+        <v>Instrument/default/Ticker</v>
       </c>
       <c r="G22" s="18" t="b">
         <v>0</v>
@@ -7067,13 +7078,13 @@
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
       <c r="E23" s="36" t="str">
-        <v>Wertpapier</v>
+        <v>Figi</v>
       </c>
       <c r="F23" s="18" t="str">
-        <v>Instrument/default/Wertpapier</v>
+        <v>Instrument/default/Figi</v>
       </c>
       <c r="G23" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -7089,13 +7100,13 @@
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="36" t="str">
-        <v>LusidInstrumentId</v>
+        <v>RIC</v>
       </c>
       <c r="F24" s="18" t="str">
-        <v>Instrument/default/LusidInstrumentId</v>
+        <v>Instrument/default/RIC</v>
       </c>
       <c r="G24" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -7110,10 +7121,10 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
       <c r="E25" s="36" t="str">
-        <v>QuotePermId</v>
+        <v>LusidInstrumentId</v>
       </c>
       <c r="F25" s="18" t="str">
-        <v>Instrument/default/QuotePermId</v>
+        <v>Instrument/default/LusidInstrumentId</v>
       </c>
       <c r="G25" s="18" t="b">
         <v>1</v>
@@ -7148,10 +7159,10 @@
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
       <c r="E27" s="36" t="str">
-        <v>Figi</v>
+        <v>Currency</v>
       </c>
       <c r="F27" s="18" t="str">
-        <v>Instrument/default/Figi</v>
+        <v>Instrument/default/Currency</v>
       </c>
       <c r="G27" s="18" t="b">
         <v>1</v>
@@ -7167,13 +7178,13 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="36" t="str">
-        <v>RIC</v>
+        <v>QuotePermId</v>
       </c>
       <c r="F28" s="18" t="str">
-        <v>Instrument/default/RIC</v>
+        <v>Instrument/default/QuotePermId</v>
       </c>
       <c r="G28" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -7186,13 +7197,13 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="36" t="str">
-        <v>EdiKey</v>
+        <v>[More...]</v>
       </c>
       <c r="F29" s="18" t="str">
-        <v>Instrument/default/EdiKey</v>
-      </c>
-      <c r="G29" s="18" t="b">
-        <v>1</v>
+        <v>[More...]</v>
+      </c>
+      <c r="G29" s="18" t="str">
+        <v>[More...]</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -7245,7 +7256,7 @@
   <dimension ref="B1:K34"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7288,7 +7299,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -7314,7 +7325,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -7328,7 +7339,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -7343,7 +7354,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -7357,7 +7368,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -7371,7 +7382,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -7407,7 +7418,7 @@
     <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
       <c r="C14" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -7435,7 +7446,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -7449,7 +7460,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -7463,7 +7474,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -7489,13 +7500,13 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F20" s="33" t="s">
         <v>198</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -7507,8 +7518,8 @@
       <c r="C21" s="2"/>
       <c r="D21" s="9"/>
       <c r="E21" s="25">
-        <f ca="1">NOW()</f>
-        <v>43803.438066550923</v>
+        <f ca="1">TODAY()</f>
+        <v>43833</v>
       </c>
       <c r="F21" s="25">
         <v>43697</v>
@@ -7566,11 +7577,11 @@
       </c>
       <c r="F24" s="18" t="str">
         <f ca="1"/>
-        <v>CCY_ZZZ</v>
+        <v>CCY_AED</v>
       </c>
       <c r="G24" s="18" t="str">
         <f ca="1"/>
-        <v>ZZZ</v>
+        <v>AED</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -7589,11 +7600,11 @@
       </c>
       <c r="F25" s="18" t="str">
         <f ca="1"/>
-        <v>CCY_ALL</v>
+        <v>CCY_AFN</v>
       </c>
       <c r="G25" s="18" t="str">
         <f ca="1"/>
-        <v>ALL</v>
+        <v>AFN</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -7612,11 +7623,11 @@
       </c>
       <c r="F26" s="18" t="str">
         <f ca="1"/>
-        <v>CCY_DZD</v>
+        <v>CCY_ALL</v>
       </c>
       <c r="G26" s="18" t="str">
         <f ca="1"/>
-        <v>DZD</v>
+        <v>ALL</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -7635,11 +7646,11 @@
       </c>
       <c r="F27" s="18" t="str">
         <f ca="1"/>
-        <v>CCY_ARS</v>
+        <v>CCY_AMD</v>
       </c>
       <c r="G27" s="18" t="str">
         <f ca="1"/>
-        <v>ARS</v>
+        <v>AMD</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -7658,11 +7669,11 @@
       </c>
       <c r="F28" s="18" t="str">
         <f ca="1"/>
-        <v>CCY_AUD</v>
+        <v>CCY_ANG</v>
       </c>
       <c r="G28" s="18" t="str">
         <f ca="1"/>
-        <v>AUD</v>
+        <v>ANG</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -7675,17 +7686,17 @@
       <c r="D29" s="2">
         <v>6</v>
       </c>
-      <c r="E29" s="36" t="e">
+      <c r="E29" s="36" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F29" s="18" t="e">
+        <v/>
+      </c>
+      <c r="F29" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G29" s="18" t="e">
+        <v/>
+      </c>
+      <c r="G29" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -7698,17 +7709,17 @@
       <c r="D30" s="2">
         <v>7</v>
       </c>
-      <c r="E30" s="36" t="e">
+      <c r="E30" s="36" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F30" s="18" t="e">
+        <v/>
+      </c>
+      <c r="F30" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G30" s="18" t="e">
+        <v/>
+      </c>
+      <c r="G30" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -7721,17 +7732,17 @@
       <c r="D31" s="2">
         <v>8</v>
       </c>
-      <c r="E31" s="36" t="e">
+      <c r="E31" s="36" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F31" s="18" t="e">
+        <v/>
+      </c>
+      <c r="F31" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G31" s="18" t="e">
+        <v/>
+      </c>
+      <c r="G31" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -7744,17 +7755,17 @@
       <c r="D32" s="2">
         <v>9</v>
       </c>
-      <c r="E32" s="36" t="e">
+      <c r="E32" s="36" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F32" s="18" t="e">
+        <v/>
+      </c>
+      <c r="F32" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G32" s="18" t="e">
+        <v/>
+      </c>
+      <c r="G32" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -7767,17 +7778,17 @@
       <c r="D33" s="2">
         <v>10</v>
       </c>
-      <c r="E33" s="36" t="e">
+      <c r="E33" s="36" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F33" s="18" t="e">
+        <v/>
+      </c>
+      <c r="F33" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G33" s="18" t="e">
+        <v/>
+      </c>
+      <c r="G33" s="18" t="str">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -7861,7 +7872,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -7889,7 +7900,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -7904,7 +7915,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -7920,7 +7931,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -7935,7 +7946,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -7950,7 +7961,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -7992,7 +8003,7 @@
     <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -8022,7 +8033,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -8037,7 +8048,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -8052,7 +8063,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -8125,8 +8136,8 @@
       <c r="I21" s="33" t="str">
         <v>Figi</v>
       </c>
-      <c r="J21" s="33" t="e">
-        <v>#N/A</v>
+      <c r="J21" s="33" t="str">
+        <v/>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -8147,7 +8158,7 @@
         <v>Active</v>
       </c>
       <c r="G22" s="18" t="str">
-        <v>LUID_52QAWPO6</v>
+        <v>LUID_JENBWO5H</v>
       </c>
       <c r="H22" s="35" t="str">
         <v>Apple</v>
@@ -8155,8 +8166,8 @@
       <c r="I22" s="35" t="str">
         <v>BBG000B9XRY4</v>
       </c>
-      <c r="J22" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J22" s="52" t="str">
+        <v/>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -8177,7 +8188,7 @@
         <v>Active</v>
       </c>
       <c r="G23" s="18" t="str">
-        <v>LUID_8M11ADAC</v>
+        <v>LUID_6IOL49Q5</v>
       </c>
       <c r="H23" s="35" t="str">
         <v>JPMorgan Chase</v>
@@ -8185,8 +8196,8 @@
       <c r="I23" s="35" t="str">
         <v>BBG000DMBXR2</v>
       </c>
-      <c r="J23" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J23" s="52" t="str">
+        <v/>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -8207,7 +8218,7 @@
         <v>Active</v>
       </c>
       <c r="G24" s="18" t="str">
-        <v>LUID_4JZB9MLP</v>
+        <v>LUID_AHX7SPIA</v>
       </c>
       <c r="H24" s="35" t="str">
         <v>BP</v>
@@ -8215,8 +8226,8 @@
       <c r="I24" s="35" t="str">
         <v>BBG000C059M6</v>
       </c>
-      <c r="J24" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J24" s="52" t="str">
+        <v/>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -8237,7 +8248,7 @@
         <v>Active</v>
       </c>
       <c r="G25" s="18" t="str">
-        <v>LUID_Z03VAEWV</v>
+        <v>LUID_LNXBDXBB</v>
       </c>
       <c r="H25" s="35" t="str">
         <v>Anheuser-Busch InBev</v>
@@ -8245,8 +8256,8 @@
       <c r="I25" s="35" t="str">
         <v>BBG00DQ4YZ36</v>
       </c>
-      <c r="J25" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J25" s="52" t="str">
+        <v/>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -8267,7 +8278,7 @@
         <v>Active</v>
       </c>
       <c r="G26" s="18" t="str">
-        <v>LUID_WYX0SDPX</v>
+        <v>LUID_OQEOT1JY</v>
       </c>
       <c r="H26" s="35" t="str">
         <v>Toyota Motor</v>
@@ -8275,8 +8286,8 @@
       <c r="I26" s="35" t="str">
         <v>BBG000BCM915</v>
       </c>
-      <c r="J26" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J26" s="52" t="str">
+        <v/>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -8297,7 +8308,7 @@
         <v>Active</v>
       </c>
       <c r="G27" s="18" t="str">
-        <v>LUID_F9FDBWL0</v>
+        <v>LUID_L5UE01IN</v>
       </c>
       <c r="H27" s="35" t="str">
         <v>Volkswagen</v>
@@ -8305,8 +8316,8 @@
       <c r="I27" s="35" t="str">
         <v>BBG000BCH458</v>
       </c>
-      <c r="J27" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J27" s="52" t="str">
+        <v/>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -8327,7 +8338,7 @@
         <v>Active</v>
       </c>
       <c r="G28" s="18" t="str">
-        <v>LUID_816OBQZV</v>
+        <v>LUID_V9OX6CRE</v>
       </c>
       <c r="H28" s="35" t="str">
         <v>HSBC Holdings</v>
@@ -8335,8 +8346,8 @@
       <c r="I28" s="35" t="str">
         <v>BBG000BS1MT4</v>
       </c>
-      <c r="J28" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J28" s="52" t="str">
+        <v/>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -8356,7 +8367,7 @@
         <v>Active</v>
       </c>
       <c r="G29" s="18" t="str">
-        <v>LUID_3IPLDPSN</v>
+        <v>LUID_58EHIPFX</v>
       </c>
       <c r="H29" s="35" t="str">
         <v>Walt Disney</v>
@@ -8364,8 +8375,8 @@
       <c r="I29" s="35" t="str">
         <v>BBG000BH4R78</v>
       </c>
-      <c r="J29" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J29" s="52" t="str">
+        <v/>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -8383,7 +8394,7 @@
         <v>Active</v>
       </c>
       <c r="G30" s="18" t="str">
-        <v>LUID_UW1XTP85</v>
+        <v>LUID_230PNNYD</v>
       </c>
       <c r="H30" s="35" t="str">
         <v>Microsoft</v>
@@ -8391,8 +8402,8 @@
       <c r="I30" s="35" t="str">
         <v>BBG000BPH459</v>
       </c>
-      <c r="J30" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J30" s="52" t="str">
+        <v/>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -8410,7 +8421,7 @@
         <v>Active</v>
       </c>
       <c r="G31" s="18" t="str">
-        <v>LUID_A18IZK18</v>
+        <v>LUID_JL12HZYH</v>
       </c>
       <c r="H31" s="35" t="str">
         <v>Softbank</v>
@@ -8418,8 +8429,8 @@
       <c r="I31" s="35" t="str">
         <v>BBG000CLY2D3</v>
       </c>
-      <c r="J31" s="52" t="e">
-        <v>#N/A</v>
+      <c r="J31" s="52" t="str">
+        <v/>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -8515,7 +8526,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -8545,7 +8556,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -8561,7 +8572,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -8578,7 +8589,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -8594,7 +8605,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -8610,7 +8621,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -8667,7 +8678,7 @@
     <row r="13" spans="2:19" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -8699,7 +8710,7 @@
       <c r="C15" s="10"/>
       <c r="D15" s="2"/>
       <c r="E15" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -8715,7 +8726,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -8748,22 +8759,22 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="K18" s="8"/>
       <c r="L18" s="2"/>
@@ -8788,25 +8799,25 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="I20" s="8" t="s">
+      <c r="J20" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="K20" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -8816,7 +8827,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="9"/>
       <c r="E21" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>204</v>
@@ -8826,7 +8837,7 @@
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="50" t="str">
@@ -8855,25 +8866,25 @@
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="K23" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -8883,7 +8894,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>204</v>
@@ -8893,7 +8904,7 @@
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="50" t="str">
@@ -8934,7 +8945,7 @@
     <row r="28" spans="2:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B28" s="2"/>
       <c r="C28" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -8966,7 +8977,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -9043,11 +9054,11 @@
       <c r="I34" s="8" t="str">
         <v>Figi</v>
       </c>
-      <c r="J34" s="8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K34" s="8" t="e">
-        <v>#N/A</v>
+      <c r="J34" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K34" s="8" t="str">
+        <v/>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
@@ -9064,7 +9075,7 @@
         <v>Active</v>
       </c>
       <c r="G35" s="13" t="str">
-        <v>LUID_52QAWPO6</v>
+        <v>LUID_JENBWO5H</v>
       </c>
       <c r="H35" s="16" t="str">
         <v>Apple</v>
@@ -9072,11 +9083,11 @@
       <c r="I35" s="16" t="str">
         <v>BBG000B9XRY4</v>
       </c>
-      <c r="J35" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K35" s="17" t="e">
-        <v>#N/A</v>
+      <c r="J35" s="17" t="str">
+        <v/>
+      </c>
+      <c r="K35" s="17" t="str">
+        <v/>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -9093,7 +9104,7 @@
         <v>Active</v>
       </c>
       <c r="G36" s="13" t="str">
-        <v>LUID_3IPLDPSN</v>
+        <v>LUID_58EHIPFX</v>
       </c>
       <c r="H36" s="16" t="str">
         <v>Walt Disney</v>
@@ -9101,11 +9112,11 @@
       <c r="I36" s="16" t="str">
         <v>BBG000BH4R78</v>
       </c>
-      <c r="J36" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K36" s="17" t="e">
-        <v>#N/A</v>
+      <c r="J36" s="17" t="str">
+        <v/>
+      </c>
+      <c r="K36" s="17" t="str">
+        <v/>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -9312,10 +9323,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:M32"/>
+  <dimension ref="B1:M33"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9361,7 +9372,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -9391,7 +9402,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -9407,7 +9418,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -9424,7 +9435,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -9440,7 +9451,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -9456,7 +9467,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -9498,7 +9509,7 @@
     <row r="13" spans="2:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -9516,7 +9527,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -9546,7 +9557,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -9576,25 +9587,25 @@
       <c r="C18" s="2"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>315</v>
-      </c>
       <c r="K18" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -9604,20 +9615,20 @@
       <c r="C19" s="2"/>
       <c r="D19" s="9"/>
       <c r="E19" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>
       <c r="K19" s="50" t="str">
         <f>_xll.flInstrumentsAdd(E18:J19)</f>
-        <v>LUID_SVI3RKHJ</v>
+        <v>LUID_8VIVIFMY</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -9653,7 +9664,7 @@
     <row r="23" spans="2:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
       <c r="C23" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -9671,7 +9682,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -9734,7 +9745,7 @@
         <v>202</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G28" s="8" t="str">
         <f t="array" ref="G28:L29">_xll.flInstrumentsLookup(F29,E29,"Instrument/default/Ticker")</f>
@@ -9750,10 +9761,10 @@
         <v>Ticker</v>
       </c>
       <c r="K28" s="8" t="str">
+        <v>Isin</v>
+      </c>
+      <c r="L28" s="8" t="str">
         <v>Figi</v>
-      </c>
-      <c r="L28" s="8" t="str">
-        <v>Isin</v>
       </c>
       <c r="M28" s="2"/>
     </row>
@@ -9762,7 +9773,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="9"/>
       <c r="E29" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>204</v>
@@ -9771,7 +9782,7 @@
         <v>Active</v>
       </c>
       <c r="H29" s="13" t="str">
-        <v>LUID_SVI3RKHJ</v>
+        <v>LUID_8VIVIFMY</v>
       </c>
       <c r="I29" s="13" t="str">
         <v>Spectre</v>
@@ -9780,10 +9791,10 @@
         <v>0</v>
       </c>
       <c r="K29" s="16" t="str">
+        <v>GB007007007B</v>
+      </c>
+      <c r="L29" s="17" t="str">
         <v>BBG007FAKECO</v>
-      </c>
-      <c r="L29" s="17" t="str">
-        <v>GB007007007B</v>
       </c>
       <c r="M29" s="2"/>
     </row>
@@ -9805,10 +9816,10 @@
       <c r="C31" s="2"/>
       <c r="D31" s="9"/>
       <c r="E31" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G31" s="18" t="str">
         <f>_xll.flInstrumentsLookup(F31,E31,"Instrument/default/Ticker")</f>
@@ -9823,12 +9834,52 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
+      <c r="G32" s="8" t="str">
+        <f t="array" ref="G32:L33">_xll.flInstrumentsLookup(F33,E33,"Instrument/default/Ticker")</f>
+        <v>State</v>
+      </c>
+      <c r="H32" s="8" t="str">
+        <v>LusidInstrumentId</v>
+      </c>
+      <c r="I32" s="8" t="str">
+        <v>Name</v>
+      </c>
+      <c r="J32" s="7" t="str">
+        <v>Ticker</v>
+      </c>
+      <c r="K32" s="8" t="str">
+        <v>Isin</v>
+      </c>
+      <c r="L32" s="8" t="str">
+        <v>Figi</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E33" s="17" t="str">
+        <f>K19</f>
+        <v>LUID_8VIVIFMY</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="G33" s="23" t="str">
+        <v>Active</v>
+      </c>
+      <c r="H33" s="23" t="str">
+        <v>LUID_8VIVIFMY</v>
+      </c>
+      <c r="I33" s="23" t="str">
+        <v>Spectre</v>
+      </c>
+      <c r="J33" s="23">
+        <v>0</v>
+      </c>
+      <c r="K33" s="23" t="str">
+        <v>GB007007007B</v>
+      </c>
+      <c r="L33" s="23" t="str">
+        <v>BBG007FAKECO</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="18">
@@ -9869,7 +9920,9 @@
   </sheetPr>
   <dimension ref="B1:N46"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9915,7 +9968,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -9945,7 +9998,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -9961,7 +10014,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -9977,7 +10030,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -9994,7 +10047,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -10010,7 +10063,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -10026,7 +10079,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -10046,7 +10099,7 @@
         <v>OK</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -10062,25 +10115,25 @@
       <c r="C13" s="2"/>
       <c r="D13" s="9"/>
       <c r="E13" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="K13" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -10089,7 +10142,7 @@
     <row r="14" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
       <c r="C14" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -10107,7 +10160,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -10125,25 +10178,25 @@
       <c r="C16" s="2"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I16" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="K16" s="6" t="s">
         <v>285</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="L16" s="6" t="str">
         <f t="array" ref="L16:L19">_xll.flPropertiesAdd(E16:K19)</f>
@@ -10157,13 +10210,13 @@
       <c r="C17" s="2"/>
       <c r="D17" s="9"/>
       <c r="E17" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F17" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>295</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>296</v>
       </c>
       <c r="H17" s="12" t="b">
         <v>0</v>
@@ -10173,13 +10226,13 @@
         <v>PlanType</v>
       </c>
       <c r="J17" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="K17" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="K17" s="15" t="s">
-        <v>288</v>
-      </c>
       <c r="L17" s="50" t="str">
-        <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/PlanType' because it already exists.</v>
+        <v>Entity already exists</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -10189,28 +10242,28 @@
       <c r="C18" s="2"/>
       <c r="D18" s="9"/>
       <c r="E18" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H18" s="42" t="b">
         <v>0</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J18" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L18" s="50" t="str">
-        <v>Error creating Property Definition 'Instrument/FinbourneBondVillains/TakeOverWorldDate' because it already exists.</v>
+        <v>Entity already exists</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -10223,25 +10276,25 @@
         <v>180</v>
       </c>
       <c r="F19" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>336</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>337</v>
       </c>
       <c r="H19" s="42" t="b">
         <v>0</v>
       </c>
       <c r="I19" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="K19" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="J19" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>338</v>
-      </c>
       <c r="L19" s="51" t="str">
-        <v>Error creating Property Definition 'Transaction/Finbourne-Examples/IsThisATestTrade' because it already exists.</v>
+        <v>Entity already exists</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -10330,7 +10383,7 @@
         <v>OK</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -10346,16 +10399,16 @@
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="G27" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>333</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="6"/>
@@ -10367,7 +10420,7 @@
     <row r="28" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B28" s="2"/>
       <c r="C28" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -10385,7 +10438,7 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -10403,19 +10456,19 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>332</v>
-      </c>
       <c r="G30" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H30" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="I30" s="33" t="s">
         <v>299</v>
-      </c>
-      <c r="I30" s="33" t="s">
-        <v>300</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -10430,20 +10483,20 @@
         <v>1</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F31" s="15" t="str">
         <f>'Add instrument'!K19</f>
-        <v>LUID_SVI3RKHJ</v>
+        <v>LUID_8VIVIFMY</v>
       </c>
       <c r="G31" s="46">
         <v>43101</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I31" s="45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J31" s="41"/>
       <c r="K31" s="50" t="str">
@@ -10536,7 +10589,7 @@
     <row r="37" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>
       <c r="C37" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -10554,7 +10607,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -10590,7 +10643,7 @@
         <v>203</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -10624,7 +10677,7 @@
         <v>202</v>
       </c>
       <c r="F42" s="8" t="str">
-        <f t="array" ref="F42:L43">_xll.flInstrumentsLookup(F40,E43:E44,H30&amp;","&amp;I30)</f>
+        <f t="array" ref="F42:L43">_xll.flInstrumentsLookup(F40,E43:E44,I30&amp;","&amp;H30)</f>
         <v>State</v>
       </c>
       <c r="G42" s="8" t="str">
@@ -10640,10 +10693,10 @@
         <v>TakeOverDate</v>
       </c>
       <c r="K42" s="8" t="str">
+        <v>Figi</v>
+      </c>
+      <c r="L42" s="8" t="str">
         <v>Isin</v>
-      </c>
-      <c r="L42" s="8" t="str">
-        <v>Figi</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -10654,13 +10707,13 @@
       <c r="D43" s="9"/>
       <c r="E43" s="15" t="str">
         <f>F31</f>
-        <v>LUID_SVI3RKHJ</v>
+        <v>LUID_8VIVIFMY</v>
       </c>
       <c r="F43" s="42" t="str">
         <v>Active</v>
       </c>
       <c r="G43" s="42" t="str">
-        <v>LUID_SVI3RKHJ</v>
+        <v>LUID_8VIVIFMY</v>
       </c>
       <c r="H43" s="41" t="str">
         <v>Spectre</v>
@@ -10672,10 +10725,10 @@
         <v>2028/12/01T00:00:00.00</v>
       </c>
       <c r="K43" s="41" t="str">
+        <v>BBG007FAKECO</v>
+      </c>
+      <c r="L43" s="50" t="str">
         <v>GB007007007B</v>
-      </c>
-      <c r="L43" s="50" t="str">
-        <v>BBG007FAKECO</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -10762,7 +10815,9 @@
   </sheetPr>
   <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10806,7 +10861,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -10838,7 +10893,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -10855,7 +10910,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -10873,7 +10928,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -10890,7 +10945,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -10907,7 +10962,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -10984,7 +11039,7 @@
     <row r="13" spans="2:21" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="2"/>
@@ -11035,7 +11090,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -11123,7 +11178,7 @@
     <row r="19" spans="2:22" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -11171,34 +11226,34 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="G21" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="I21" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>198</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21"/>
@@ -11214,7 +11269,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
       <c r="E22" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="16" t="s">
@@ -11227,7 +11282,7 @@
         <v>186</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K22" s="20">
         <v>43570</v>
@@ -11252,7 +11307,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
       <c r="E23" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="16" t="s">
@@ -11265,7 +11320,7 @@
         <v>186</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K23" s="20">
         <f>K22+1</f>
@@ -11291,7 +11346,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="16" t="s">
@@ -11304,7 +11359,7 @@
         <v>186</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K24" s="20">
         <f t="shared" ref="K24:K30" si="0">K23+1</f>
@@ -11330,7 +11385,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
       <c r="E25" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="16" t="s">
@@ -11343,7 +11398,7 @@
         <v>186</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K25" s="20">
         <f t="shared" si="0"/>
@@ -11369,7 +11424,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
       <c r="E26" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
@@ -11382,7 +11437,7 @@
         <v>186</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K26" s="20">
         <f t="shared" si="0"/>
@@ -11405,7 +11460,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
       <c r="E27" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
@@ -11418,7 +11473,7 @@
         <v>186</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K27" s="20">
         <f t="shared" si="0"/>
@@ -11441,7 +11496,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="9"/>
       <c r="E28" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
@@ -11454,7 +11509,7 @@
         <v>186</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K28" s="20">
         <f t="shared" si="0"/>
@@ -11477,7 +11532,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="9"/>
       <c r="E29" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="16" t="s">
@@ -11490,7 +11545,7 @@
         <v>186</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K29" s="20">
         <f t="shared" si="0"/>
@@ -11513,7 +11568,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="9"/>
       <c r="E30" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="16" t="s">
@@ -11526,7 +11581,7 @@
         <v>186</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K30" s="20">
         <f t="shared" si="0"/>
@@ -11627,7 +11682,9 @@
   </sheetPr>
   <dimension ref="B1:V34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22:J31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11671,7 +11728,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -11703,7 +11760,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -11720,7 +11777,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -11738,7 +11795,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -11755,7 +11812,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -11772,7 +11829,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -11817,7 +11874,7 @@
     <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="2"/>
@@ -11854,7 +11911,7 @@
         <v>184</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>183</v>
@@ -11912,7 +11969,7 @@
     <row r="19" spans="2:22" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -11946,31 +12003,31 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="G21" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="I21" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>198</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N21" s="2"/>
       <c r="T21" s="19"/>
@@ -11982,7 +12039,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
       <c r="E22" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="16" t="s">
@@ -11995,7 +12052,7 @@
         <v>186</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K22" s="20">
         <v>43570</v>
@@ -12015,7 +12072,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="9"/>
       <c r="E23" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="16" t="s">
@@ -12028,7 +12085,7 @@
         <v>186</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K23" s="20">
         <v>43571</v>
@@ -12048,7 +12105,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="16" t="s">
@@ -12061,7 +12118,7 @@
         <v>186</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K24" s="20">
         <v>43572</v>
@@ -12081,7 +12138,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
       <c r="E25" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="16" t="s">
@@ -12094,7 +12151,7 @@
         <v>186</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K25" s="20">
         <v>43573</v>
@@ -12115,7 +12172,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
       <c r="E26" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
@@ -12128,7 +12185,7 @@
         <v>186</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K26" s="20">
         <v>43574</v>
@@ -12146,7 +12203,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="9"/>
       <c r="E27" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
@@ -12159,7 +12216,7 @@
         <v>186</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K27" s="20">
         <v>43575</v>
@@ -12177,7 +12234,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="9"/>
       <c r="E28" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
@@ -12190,7 +12247,7 @@
         <v>186</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K28" s="20">
         <v>43576</v>
@@ -12208,7 +12265,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="9"/>
       <c r="E29" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="16" t="s">
@@ -12221,7 +12278,7 @@
         <v>186</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K29" s="20">
         <v>43577</v>
@@ -12239,7 +12296,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="9"/>
       <c r="E30" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="16" t="s">
@@ -12252,7 +12309,7 @@
         <v>186</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K30" s="20">
         <v>43578</v>
@@ -12270,7 +12327,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="9"/>
       <c r="E31" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="16" t="s">
@@ -12283,7 +12340,7 @@
         <v>186</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="K31" s="20">
         <v>43579</v>
@@ -12331,12 +12388,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12566,19 +12624,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F07F7B26-A8FB-44CC-BC1A-494CF9683469}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
+    <ds:schemaRef ds:uri="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12604,19 +12671,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F07F7B26-A8FB-44CC-BC1A-494CF9683469}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
-    <ds:schemaRef ds:uri="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>